<commit_message>
goliatt sáb dez 11 00:09:57 -03 2021
</commit_message>
<xml_diff>
--- a/table_best_models____spi-3__test.xlsx
+++ b/table_best_models____spi-3__test.xlsx
@@ -426,22 +426,22 @@
         <v>0.798426952</v>
       </c>
       <c r="B2">
-        <v>0.8570327669061935</v>
+        <v>0.8570327671020751</v>
       </c>
       <c r="C2">
-        <v>0.8674250062065214</v>
+        <v>0.8674250061198436</v>
       </c>
       <c r="D2">
-        <v>0.867085419348429</v>
+        <v>0.8670854193478963</v>
       </c>
       <c r="E2">
-        <v>0.8659723676718361</v>
+        <v>0.8659723676718362</v>
       </c>
       <c r="F2">
-        <v>0.8670463417751291</v>
+        <v>0.867046342060002</v>
       </c>
       <c r="G2">
-        <v>0.8592882910984204</v>
+        <v>0.8592882910984092</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -449,22 +449,22 @@
         <v>-0.135008744</v>
       </c>
       <c r="B3">
-        <v>0.7326825153109942</v>
+        <v>0.7326825141436214</v>
       </c>
       <c r="C3">
-        <v>0.766074904899262</v>
+        <v>0.7660749047608373</v>
       </c>
       <c r="D3">
-        <v>0.7170747516094111</v>
+        <v>0.7170747516091714</v>
       </c>
       <c r="E3">
-        <v>0.7184550245767005</v>
+        <v>0.7184550245767007</v>
       </c>
       <c r="F3">
-        <v>0.7593774095256962</v>
+        <v>0.7593774097772397</v>
       </c>
       <c r="G3">
-        <v>0.7523822066406652</v>
+        <v>0.7523822066406555</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -472,22 +472,22 @@
         <v>0.483128577</v>
       </c>
       <c r="B4">
-        <v>0.1599370752091069</v>
+        <v>0.159937075596327</v>
       </c>
       <c r="C4">
-        <v>0.2109950895175152</v>
+        <v>0.2109950894471056</v>
       </c>
       <c r="D4">
-        <v>0.1805269018647987</v>
+        <v>0.1805269018647896</v>
       </c>
       <c r="E4">
-        <v>0.1815890235630253</v>
+        <v>0.1815890235630254</v>
       </c>
       <c r="F4">
-        <v>0.2069589467509748</v>
+        <v>0.2069589468302485</v>
       </c>
       <c r="G4">
-        <v>0.203862447999262</v>
+        <v>0.2038624479992588</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -495,22 +495,22 @@
         <v>0.358803155</v>
       </c>
       <c r="B5">
-        <v>-0.422666630974163</v>
+        <v>-0.4226666300367006</v>
       </c>
       <c r="C5">
-        <v>-0.3115414410597218</v>
+        <v>-0.3115414410878165</v>
       </c>
       <c r="D5">
-        <v>-0.3805194157062556</v>
+        <v>-0.3805194157057444</v>
       </c>
       <c r="E5">
-        <v>-0.3812088072526029</v>
+        <v>-0.3812088072526028</v>
       </c>
       <c r="F5">
-        <v>-0.3145528385420044</v>
+        <v>-0.3145528386299085</v>
       </c>
       <c r="G5">
-        <v>-0.3147940136636524</v>
+        <v>-0.3147940136636487</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -518,22 +518,22 @@
         <v>0.9297649529999999</v>
       </c>
       <c r="B6">
-        <v>0.1366489189338796</v>
+        <v>0.1366489192602485</v>
       </c>
       <c r="C6">
-        <v>0.2161612460234723</v>
+        <v>0.2161612459445032</v>
       </c>
       <c r="D6">
-        <v>0.1465630873628219</v>
+        <v>0.1465630873630199</v>
       </c>
       <c r="E6">
-        <v>0.1510350243694587</v>
+        <v>0.1510350243694589</v>
       </c>
       <c r="F6">
-        <v>0.2110634079315908</v>
+        <v>0.2110634080120473</v>
       </c>
       <c r="G6">
-        <v>0.208132795746566</v>
+        <v>0.2081327957465628</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -541,22 +541,22 @@
         <v>-0.343866365</v>
       </c>
       <c r="B7">
-        <v>-0.605568517847453</v>
+        <v>-0.6055685168215885</v>
       </c>
       <c r="C7">
-        <v>-0.5478437317968556</v>
+        <v>-0.5478437317397367</v>
       </c>
       <c r="D7">
-        <v>-0.5873153748262638</v>
+        <v>-0.5873153748257482</v>
       </c>
       <c r="E7">
-        <v>-0.5777404405979616</v>
+        <v>-0.5777404405979614</v>
       </c>
       <c r="F7">
-        <v>-0.5395843898001192</v>
+        <v>-0.5395843899572571</v>
       </c>
       <c r="G7">
-        <v>-0.5423760231806951</v>
+        <v>-0.542376023180689</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -564,22 +564,22 @@
         <v>-0.394869887</v>
       </c>
       <c r="B8">
-        <v>-0.3544013528870553</v>
+        <v>-0.354401351100021</v>
       </c>
       <c r="C8">
-        <v>-0.2562379889659018</v>
+        <v>-0.25623798896717</v>
       </c>
       <c r="D8">
-        <v>-0.2911052084766264</v>
+        <v>-0.2911052084763237</v>
       </c>
       <c r="E8">
-        <v>-0.2893305255051054</v>
+        <v>-0.2893305255051053</v>
       </c>
       <c r="F8">
-        <v>-0.2571016599171884</v>
+        <v>-0.2571016599835869</v>
       </c>
       <c r="G8">
-        <v>-0.2565996292859046</v>
+        <v>-0.256599629285902</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -587,22 +587,22 @@
         <v>0.124976886</v>
       </c>
       <c r="B9">
-        <v>0.4065369388324497</v>
+        <v>0.4065369392719085</v>
       </c>
       <c r="C9">
-        <v>0.4550571594302947</v>
+        <v>0.4550571593413335</v>
       </c>
       <c r="D9">
-        <v>0.4436391972448822</v>
+        <v>0.443639197244627</v>
       </c>
       <c r="E9">
-        <v>0.4430181914949464</v>
+        <v>0.4430181914949466</v>
       </c>
       <c r="F9">
-        <v>0.4512238385970701</v>
+        <v>0.4512238387534177</v>
       </c>
       <c r="G9">
-        <v>0.4462374925194673</v>
+        <v>0.4462374925194611</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -610,22 +610,22 @@
         <v>0.714385868</v>
       </c>
       <c r="B10">
-        <v>0.8459672688667423</v>
+        <v>0.8459672685817484</v>
       </c>
       <c r="C10">
-        <v>0.8863712727299621</v>
+        <v>0.8863712726228958</v>
       </c>
       <c r="D10">
-        <v>0.8804605020657794</v>
+        <v>0.8804605020652532</v>
       </c>
       <c r="E10">
-        <v>0.8796607527224343</v>
+        <v>0.8796607527224344</v>
       </c>
       <c r="F10">
-        <v>0.8852831167770526</v>
+        <v>0.8852831170688441</v>
       </c>
       <c r="G10">
-        <v>0.8761127367562926</v>
+        <v>0.876112736756281</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -633,22 +633,22 @@
         <v>0.495936019</v>
       </c>
       <c r="B11">
-        <v>0.5114182908847229</v>
+        <v>0.5114182901811332</v>
       </c>
       <c r="C11">
-        <v>0.5326541336362253</v>
+        <v>0.5326541335343883</v>
       </c>
       <c r="D11">
-        <v>0.5056704980131439</v>
+        <v>0.5056704980129281</v>
       </c>
       <c r="E11">
-        <v>0.5061906675405067</v>
+        <v>0.5061906675405068</v>
       </c>
       <c r="F11">
-        <v>0.527606065430581</v>
+        <v>0.5276060656096382</v>
       </c>
       <c r="G11">
-        <v>0.5225599813036714</v>
+        <v>0.5225599813036644</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -656,22 +656,22 @@
         <v>-1.049232267</v>
       </c>
       <c r="B12">
-        <v>-0.8549446300139482</v>
+        <v>-0.8549446305690328</v>
       </c>
       <c r="C12">
-        <v>-0.8548170792389924</v>
+        <v>-0.8548170791291492</v>
       </c>
       <c r="D12">
-        <v>-0.8861227154469821</v>
+        <v>-0.8861227154463175</v>
       </c>
       <c r="E12">
         <v>-0.8920379021151954</v>
       </c>
       <c r="F12">
-        <v>-0.8584596349668585</v>
+        <v>-0.8584596352192811</v>
       </c>
       <c r="G12">
-        <v>-0.8441335123158528</v>
+        <v>-0.8441335123158428</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -679,22 +679,22 @@
         <v>-0.962528123</v>
       </c>
       <c r="B13">
-        <v>-0.5508499191351595</v>
+        <v>-0.5508499193587389</v>
       </c>
       <c r="C13">
-        <v>-0.558830444886909</v>
+        <v>-0.5588304447962913</v>
       </c>
       <c r="D13">
-        <v>-0.6087795053264133</v>
+        <v>-0.608779505325819</v>
       </c>
       <c r="E13">
-        <v>-0.6098169651145662</v>
+        <v>-0.609816965114566</v>
       </c>
       <c r="F13">
-        <v>-0.5558074251419799</v>
+        <v>-0.5558074253001822</v>
       </c>
       <c r="G13">
-        <v>-0.5498462501739286</v>
+        <v>-0.5498462501739224</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -702,22 +702,22 @@
         <v>-0.823266309</v>
       </c>
       <c r="B14">
-        <v>-0.5387245462156625</v>
+        <v>-0.5387245457306077</v>
       </c>
       <c r="C14">
-        <v>-0.5550114420122587</v>
+        <v>-0.5550114419508775</v>
       </c>
       <c r="D14">
-        <v>-0.5556809834799619</v>
+        <v>-0.5556809834796582</v>
       </c>
       <c r="E14">
-        <v>-0.560350077502765</v>
+        <v>-0.5603500775027648</v>
       </c>
       <c r="F14">
-        <v>-0.5650099645983662</v>
+        <v>-0.56500996475396</v>
       </c>
       <c r="G14">
-        <v>-0.5490960969727708</v>
+        <v>-0.5490960969727648</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -725,22 +725,22 @@
         <v>-0.566899673</v>
       </c>
       <c r="B15">
-        <v>-0.5535699574788996</v>
+        <v>-0.553569955843472</v>
       </c>
       <c r="C15">
-        <v>-0.4900207761069212</v>
+        <v>-0.4900207760677317</v>
       </c>
       <c r="D15">
-        <v>-0.5216365655214071</v>
+        <v>-0.521636565520975</v>
       </c>
       <c r="E15">
         <v>-0.5372071996177721</v>
       </c>
       <c r="F15">
-        <v>-0.5050242795502015</v>
+        <v>-0.5050242796887064</v>
       </c>
       <c r="G15">
-        <v>-0.4863775757637694</v>
+        <v>-0.4863775757637639</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -748,22 +748,22 @@
         <v>1.061843082</v>
       </c>
       <c r="B16">
-        <v>0.8567354315799662</v>
+        <v>0.8567354323737162</v>
       </c>
       <c r="C16">
-        <v>0.9236299545935833</v>
+        <v>0.9236299545167342</v>
       </c>
       <c r="D16">
-        <v>0.9431110412198056</v>
+        <v>0.9431110412191371</v>
       </c>
       <c r="E16">
-        <v>0.942245690758327</v>
+        <v>0.9422456907583271</v>
       </c>
       <c r="F16">
-        <v>0.926818369117928</v>
+        <v>0.9268183694219724</v>
       </c>
       <c r="G16">
-        <v>0.916591442995258</v>
+        <v>0.9165914429952459</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -771,22 +771,22 @@
         <v>1.223874814</v>
       </c>
       <c r="B17">
-        <v>1.104143636505469</v>
+        <v>1.10414363773598</v>
       </c>
       <c r="C17">
-        <v>1.160127196468206</v>
+        <v>1.160127196405216</v>
       </c>
       <c r="D17">
-        <v>1.191775102044087</v>
+        <v>1.191775102043232</v>
       </c>
       <c r="E17">
         <v>1.1901963138264</v>
       </c>
       <c r="F17">
-        <v>1.166977315555881</v>
+        <v>1.166977315935523</v>
       </c>
       <c r="G17">
-        <v>1.154804837335865</v>
+        <v>1.154804837335849</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -794,22 +794,22 @@
         <v>1.243571118</v>
       </c>
       <c r="B18">
-        <v>1.047311309591341</v>
+        <v>1.047311311849136</v>
       </c>
       <c r="C18">
-        <v>1.094528800451252</v>
+        <v>1.094528800430761</v>
       </c>
       <c r="D18">
-        <v>1.15188715665152</v>
+        <v>1.151887156650582</v>
       </c>
       <c r="E18">
         <v>1.150135093326716</v>
       </c>
       <c r="F18">
-        <v>1.105520168659705</v>
+        <v>1.10552016901935</v>
       </c>
       <c r="G18">
-        <v>1.093607344005224</v>
+        <v>1.09360734400521</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -817,22 +817,22 @@
         <v>-1.371414383</v>
       </c>
       <c r="B19">
-        <v>-1.098086676977471</v>
+        <v>-1.098086678711034</v>
       </c>
       <c r="C19">
-        <v>-1.153627873929329</v>
+        <v>-1.153627873825032</v>
       </c>
       <c r="D19">
-        <v>-1.15463395587024</v>
+        <v>-1.154633955869579</v>
       </c>
       <c r="E19">
         <v>-1.153833321743734</v>
       </c>
       <c r="F19">
-        <v>-1.155258192325818</v>
+        <v>-1.155258192675071</v>
       </c>
       <c r="G19">
-        <v>-1.143856610615345</v>
+        <v>-1.143856610615331</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -840,22 +840,22 @@
         <v>-1.6161627</v>
       </c>
       <c r="B20">
-        <v>-1.313066484620561</v>
+        <v>-1.313066484048699</v>
       </c>
       <c r="C20">
-        <v>-1.283338494725228</v>
+        <v>-1.283338494593717</v>
       </c>
       <c r="D20">
-        <v>-1.294166590443124</v>
+        <v>-1.294166590442324</v>
       </c>
       <c r="E20">
         <v>-1.29408406982016</v>
       </c>
       <c r="F20">
-        <v>-1.284311626698529</v>
+        <v>-1.284311627088639</v>
       </c>
       <c r="G20">
-        <v>-1.270845046119568</v>
+        <v>-1.270845046119552</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -863,22 +863,22 @@
         <v>-1.663613601</v>
       </c>
       <c r="B21">
-        <v>-1.328883069352831</v>
+        <v>-1.328883067250665</v>
       </c>
       <c r="C21">
-        <v>-1.246902318392439</v>
+        <v>-1.246902318176336</v>
       </c>
       <c r="D21">
-        <v>-1.290393136072034</v>
+        <v>-1.290393136071035</v>
       </c>
       <c r="E21">
         <v>-1.292109535285898</v>
       </c>
       <c r="F21">
-        <v>-1.239262440970175</v>
+        <v>-1.239262441344044</v>
       </c>
       <c r="G21">
-        <v>-1.22546047253359</v>
+        <v>-1.225460472533575</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -886,22 +886,22 @@
         <v>-0.39083508</v>
       </c>
       <c r="B22">
-        <v>-0.4714463938754819</v>
+        <v>-0.4714463925043804</v>
       </c>
       <c r="C22">
-        <v>-0.3902814283896922</v>
+        <v>-0.3902814283717299</v>
       </c>
       <c r="D22">
-        <v>-0.4298942636060505</v>
+        <v>-0.4298942636056386</v>
       </c>
       <c r="E22">
-        <v>-0.4257710583309521</v>
+        <v>-0.425771058330952</v>
       </c>
       <c r="F22">
-        <v>-0.3891915143313232</v>
+        <v>-0.3891915144401171</v>
       </c>
       <c r="G22">
-        <v>-0.3887655102598254</v>
+        <v>-0.3887655102598211</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -909,22 +909,22 @@
         <v>-1.294350414</v>
       </c>
       <c r="B23">
-        <v>-1.351254409893005</v>
+        <v>-1.351254409315158</v>
       </c>
       <c r="C23">
-        <v>-1.317022201313508</v>
+        <v>-1.317022201063619</v>
       </c>
       <c r="D23">
-        <v>-1.355119067496532</v>
+        <v>-1.355119067495509</v>
       </c>
       <c r="E23">
         <v>-1.259302186063251</v>
       </c>
       <c r="F23">
-        <v>-1.209489839655806</v>
+        <v>-1.209489840054009</v>
       </c>
       <c r="G23">
-        <v>-1.292098446580052</v>
+        <v>-1.292098446580037</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -932,22 +932,22 @@
         <v>-1.735350123</v>
       </c>
       <c r="B24">
-        <v>-1.730053202658695</v>
+        <v>-1.73005320125318</v>
       </c>
       <c r="C24">
-        <v>-1.650744240711906</v>
+        <v>-1.650744240412817</v>
       </c>
       <c r="D24">
-        <v>-1.681349034672963</v>
+        <v>-1.681349034671773</v>
       </c>
       <c r="E24">
         <v>-1.668905473279308</v>
       </c>
       <c r="F24">
-        <v>-1.624475120625088</v>
+        <v>-1.624475121125265</v>
       </c>
       <c r="G24">
-        <v>-1.621006673851335</v>
+        <v>-1.621006673851315</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -955,22 +955,22 @@
         <v>-1.464171309</v>
       </c>
       <c r="B25">
-        <v>-1.312122706353019</v>
+        <v>-1.31212270298792</v>
       </c>
       <c r="C25">
-        <v>-1.146334238943616</v>
+        <v>-1.146334238788492</v>
       </c>
       <c r="D25">
-        <v>-1.195889426589656</v>
+        <v>-1.195889426588707</v>
       </c>
       <c r="E25">
         <v>-0.9958322199963734</v>
       </c>
       <c r="F25">
-        <v>-1.003446149724364</v>
+        <v>-1.003446150075503</v>
       </c>
       <c r="G25">
-        <v>-1.131205458463125</v>
+        <v>-1.131205458463111</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -978,22 +978,22 @@
         <v>-1.138267628</v>
       </c>
       <c r="B26">
-        <v>-1.287163796411253</v>
+        <v>-1.287163792983685</v>
       </c>
       <c r="C26">
-        <v>-1.127386481780526</v>
+        <v>-1.127386481620193</v>
       </c>
       <c r="D26">
-        <v>-1.178561800767946</v>
+        <v>-1.178561800766996</v>
       </c>
       <c r="E26">
         <v>-1.190924023452542</v>
       </c>
       <c r="F26">
-        <v>-1.130831576921961</v>
+        <v>-1.130831577260678</v>
       </c>
       <c r="G26">
-        <v>-1.111688043998515</v>
+        <v>-1.111688043998501</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1001,22 +1001,22 @@
         <v>-0.231935471</v>
       </c>
       <c r="B27">
-        <v>-0.2593559483896017</v>
+        <v>-0.2593559476433276</v>
       </c>
       <c r="C27">
-        <v>-0.1947111996270687</v>
+        <v>-0.1947111996547763</v>
       </c>
       <c r="D27">
-        <v>-0.229798547768077</v>
+        <v>-0.2297985477678169</v>
       </c>
       <c r="E27">
         <v>-0.2253356024711775</v>
       </c>
       <c r="F27">
-        <v>-0.1972479020295121</v>
+        <v>-0.1972479020788469</v>
       </c>
       <c r="G27">
-        <v>-0.19779268329743</v>
+        <v>-0.197792683297428</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1024,22 +1024,22 @@
         <v>-1.071257154</v>
       </c>
       <c r="B28">
-        <v>-1.214233516307518</v>
+        <v>-1.21423351701524</v>
       </c>
       <c r="C28">
-        <v>-1.238894224721659</v>
+        <v>-1.238894224575838</v>
       </c>
       <c r="D28">
-        <v>-1.246925960817805</v>
+        <v>-1.24692596081704</v>
       </c>
       <c r="E28">
         <v>-1.247204607350994</v>
       </c>
       <c r="F28">
-        <v>-1.238365552152103</v>
+        <v>-1.238365552526167</v>
       </c>
       <c r="G28">
-        <v>-1.224842760852716</v>
+        <v>-1.224842760852701</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1047,22 +1047,22 @@
         <v>-0.788753691</v>
       </c>
       <c r="B29">
-        <v>-0.7057312823817345</v>
+        <v>-0.7057312816562966</v>
       </c>
       <c r="C29">
-        <v>-0.6705173138216989</v>
+        <v>-0.6705173137256708</v>
       </c>
       <c r="D29">
-        <v>-0.7178687858308674</v>
+        <v>-0.7178687858302228</v>
       </c>
       <c r="E29">
-        <v>-0.720398079284819</v>
+        <v>-0.7203980792848189</v>
       </c>
       <c r="F29">
-        <v>-0.6692234085683779</v>
+        <v>-0.6692234087625388</v>
       </c>
       <c r="G29">
-        <v>-0.6610867186662587</v>
+        <v>-0.661086718666251</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1070,22 +1070,22 @@
         <v>0.168216722</v>
       </c>
       <c r="B30">
-        <v>0.2964061173180312</v>
+        <v>0.2964061175682076</v>
       </c>
       <c r="C30">
-        <v>0.3359678814323325</v>
+        <v>0.3359678813561835</v>
       </c>
       <c r="D30">
-        <v>0.2847304034400414</v>
+        <v>0.2847304034400726</v>
       </c>
       <c r="E30">
-        <v>0.3015053526123817</v>
+        <v>0.301505352612382</v>
       </c>
       <c r="F30">
-        <v>0.3331286981069552</v>
+        <v>0.3331286982271702</v>
       </c>
       <c r="G30">
-        <v>0.3283703672519007</v>
+        <v>0.3283703672518958</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1093,22 +1093,22 @@
         <v>0.589617249</v>
       </c>
       <c r="B31">
-        <v>1.068030720844713</v>
+        <v>1.068030720368563</v>
       </c>
       <c r="C31">
-        <v>1.106263044480856</v>
+        <v>1.106263044351173</v>
       </c>
       <c r="D31">
-        <v>1.098698030924725</v>
+        <v>1.098698030924074</v>
       </c>
       <c r="E31">
         <v>1.096380667200003</v>
       </c>
       <c r="F31">
-        <v>1.103776647176837</v>
+        <v>1.103776647539465</v>
       </c>
       <c r="G31">
-        <v>1.093866850813675</v>
+        <v>1.09386685081366</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1116,22 +1116,22 @@
         <v>0.34764818</v>
       </c>
       <c r="B32">
-        <v>0.8119551483094981</v>
+        <v>0.8119551479412531</v>
       </c>
       <c r="C32">
-        <v>0.8429678233871636</v>
+        <v>0.8429678232674723</v>
       </c>
       <c r="D32">
-        <v>0.8287522308711528</v>
+        <v>0.8287522308706857</v>
       </c>
       <c r="E32">
-        <v>0.8269665947424443</v>
+        <v>0.8269665947424445</v>
       </c>
       <c r="F32">
-        <v>0.8387231487448393</v>
+        <v>0.8387231490240649</v>
       </c>
       <c r="G32">
-        <v>0.8313367682177035</v>
+        <v>0.8313367682176924</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1139,22 +1139,22 @@
         <v>-1.151348471</v>
       </c>
       <c r="B33">
-        <v>-0.3395585296006845</v>
+        <v>-0.3395585291620783</v>
       </c>
       <c r="C33">
-        <v>-0.3195777983870233</v>
+        <v>-0.3195777983912563</v>
       </c>
       <c r="D33">
-        <v>-0.3387822063410001</v>
+        <v>-0.3387822063407494</v>
       </c>
       <c r="E33">
         <v>-0.3398878879651326</v>
       </c>
       <c r="F33">
-        <v>-0.3240468483742153</v>
+        <v>-0.3240468484612157</v>
       </c>
       <c r="G33">
-        <v>-0.320321545997156</v>
+        <v>-0.3203215459971525</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1162,22 +1162,22 @@
         <v>-0.696093006</v>
       </c>
       <c r="B34">
-        <v>-0.748906111358869</v>
+        <v>-0.7489061106402813</v>
       </c>
       <c r="C34">
-        <v>-0.7126815279148407</v>
+        <v>-0.7126815278583926</v>
       </c>
       <c r="D34">
-        <v>-0.73275034525908</v>
+        <v>-0.7327503452585801</v>
       </c>
       <c r="E34">
-        <v>-0.7445358600045779</v>
+        <v>-0.7445358600045778</v>
       </c>
       <c r="F34">
-        <v>-0.7285928224657595</v>
+        <v>-0.7285928226752461</v>
       </c>
       <c r="G34">
-        <v>-0.7074657276202013</v>
+        <v>-0.7074657276201931</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1185,22 +1185,22 @@
         <v>-0.726012958</v>
       </c>
       <c r="B35">
-        <v>-0.5187230049141336</v>
+        <v>-0.5187230041998776</v>
       </c>
       <c r="C35">
-        <v>-0.4822834272984354</v>
+        <v>-0.4822834272884639</v>
       </c>
       <c r="D35">
-        <v>-0.4909911580287177</v>
+        <v>-0.4909911580284282</v>
       </c>
       <c r="E35">
-        <v>-0.4889364388949532</v>
+        <v>-0.4889364388949533</v>
       </c>
       <c r="F35">
-        <v>-0.4826126073562393</v>
+        <v>-0.4826126074950333</v>
       </c>
       <c r="G35">
-        <v>-0.4817098444962473</v>
+        <v>-0.4817098444962419</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1208,22 +1208,22 @@
         <v>-0.087224411</v>
       </c>
       <c r="B36">
-        <v>-0.2709417023955272</v>
+        <v>-0.2709417015515872</v>
       </c>
       <c r="C36">
-        <v>-0.23497253229086</v>
+        <v>-0.2349725323167318</v>
       </c>
       <c r="D36">
-        <v>-0.2288862305550177</v>
+        <v>-0.228886230554961</v>
       </c>
       <c r="E36">
-        <v>-0.2285303430677051</v>
+        <v>-0.2285303430677052</v>
       </c>
       <c r="F36">
-        <v>-0.2379633762296101</v>
+        <v>-0.237963376291208</v>
       </c>
       <c r="G36">
-        <v>-0.2379035261165206</v>
+        <v>-0.2379035261165182</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1231,22 +1231,22 @@
         <v>-1.025152274</v>
       </c>
       <c r="B37">
-        <v>-0.779285256741122</v>
+        <v>-0.7792852571960617</v>
       </c>
       <c r="C37">
-        <v>-0.7977091661113145</v>
+        <v>-0.7977091660328214</v>
       </c>
       <c r="D37">
-        <v>-0.80647538249416</v>
+        <v>-0.8064753824936667</v>
       </c>
       <c r="E37">
-        <v>-0.8113772313908285</v>
+        <v>-0.8113772313908286</v>
       </c>
       <c r="F37">
-        <v>-0.807348609692684</v>
+        <v>-0.8073486099274139</v>
       </c>
       <c r="G37">
-        <v>-0.7902624739898415</v>
+        <v>-0.7902624739898323</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1254,22 +1254,22 @@
         <v>-1.065636548</v>
       </c>
       <c r="B38">
-        <v>-0.9175001847433057</v>
+        <v>-0.9175001852746184</v>
       </c>
       <c r="C38">
-        <v>-0.9444270819069437</v>
+        <v>-0.9444270817803803</v>
       </c>
       <c r="D38">
-        <v>-0.9622365604700225</v>
+        <v>-0.9622365604693761</v>
       </c>
       <c r="E38">
         <v>-0.9639542619152779</v>
       </c>
       <c r="F38">
-        <v>-0.9438475217110764</v>
+        <v>-0.9438475219908058</v>
       </c>
       <c r="G38">
-        <v>-0.9320792423529147</v>
+        <v>-0.9320792423529037</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1277,22 +1277,22 @@
         <v>-1.658517568</v>
       </c>
       <c r="B39">
-        <v>-0.9921205708043189</v>
+        <v>-0.9921205694088507</v>
       </c>
       <c r="C39">
-        <v>-0.9599469516225309</v>
+        <v>-0.9599469514526012</v>
       </c>
       <c r="D39">
-        <v>-1.004865794004977</v>
+        <v>-1.004865794004151</v>
       </c>
       <c r="E39">
         <v>-1.005605574007114</v>
       </c>
       <c r="F39">
-        <v>-0.9530528555369523</v>
+        <v>-0.9530528558203429</v>
       </c>
       <c r="G39">
-        <v>-0.9430513160342286</v>
+        <v>-0.9430513160342175</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1300,22 +1300,22 @@
         <v>0.670350201</v>
       </c>
       <c r="B40">
-        <v>0.3715777945962195</v>
+        <v>0.371577793643929</v>
       </c>
       <c r="C40">
-        <v>0.3729479701139549</v>
+        <v>0.372947970033949</v>
       </c>
       <c r="D40">
-        <v>0.357505640525817</v>
+        <v>0.3575056405256379</v>
       </c>
       <c r="E40">
         <v>0.358251700435803</v>
       </c>
       <c r="F40">
-        <v>0.3693166366967808</v>
+        <v>0.3693166368247627</v>
       </c>
       <c r="G40">
-        <v>0.3649757325805799</v>
+        <v>0.3649757325805749</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1323,22 +1323,22 @@
         <v>0.58174072</v>
       </c>
       <c r="B41">
-        <v>0.384771806246977</v>
+        <v>0.384771805074932</v>
       </c>
       <c r="C41">
-        <v>0.3810728669278737</v>
+        <v>0.381072866841321</v>
       </c>
       <c r="D41">
-        <v>0.3590180041028845</v>
+        <v>0.3590180041027327</v>
       </c>
       <c r="E41">
-        <v>0.35951951287785</v>
+        <v>0.3595195128778501</v>
       </c>
       <c r="F41">
-        <v>0.3750690622504071</v>
+        <v>0.3750690623814169</v>
       </c>
       <c r="G41">
-        <v>0.3724216873541102</v>
+        <v>0.3724216873541051</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1346,22 +1346,22 @@
         <v>1.034492187</v>
       </c>
       <c r="B42">
-        <v>0.6990552409769119</v>
+        <v>0.6990552402781258</v>
       </c>
       <c r="C42">
-        <v>0.7121944759475738</v>
+        <v>0.712194475848672</v>
       </c>
       <c r="D42">
-        <v>0.7046705388878163</v>
+        <v>0.7046705388873978</v>
       </c>
       <c r="E42">
-        <v>0.7039630711949219</v>
+        <v>0.7039630711949217</v>
       </c>
       <c r="F42">
-        <v>0.7097799559730118</v>
+        <v>0.7097799562094962</v>
       </c>
       <c r="G42">
-        <v>0.7026052882596963</v>
+        <v>0.7026052882596869</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1369,22 +1369,22 @@
         <v>-0.330510864</v>
       </c>
       <c r="B43">
-        <v>-0.3090539216096562</v>
+        <v>-0.3090539206985012</v>
       </c>
       <c r="C43">
-        <v>-0.2664560678122866</v>
+        <v>-0.2664560677873326</v>
       </c>
       <c r="D43">
-        <v>-0.3206383739034048</v>
+        <v>-0.3206383739029788</v>
       </c>
       <c r="E43">
-        <v>-0.3244348244762257</v>
+        <v>-0.3244348244762256</v>
       </c>
       <c r="F43">
-        <v>-0.2682391848853534</v>
+        <v>-0.2682391849531642</v>
       </c>
       <c r="G43">
-        <v>-0.2640666716670373</v>
+        <v>-0.2640666716670347</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1392,22 +1392,22 @@
         <v>0.468647097</v>
       </c>
       <c r="B44">
-        <v>0.4212735185666343</v>
+        <v>0.421273519793997</v>
       </c>
       <c r="C44">
-        <v>0.5082044800065899</v>
+        <v>0.5082044799143509</v>
       </c>
       <c r="D44">
-        <v>0.4986448681726753</v>
+        <v>0.4986448681723796</v>
       </c>
       <c r="E44">
-        <v>0.4981425806347889</v>
+        <v>0.498142580634789</v>
       </c>
       <c r="F44">
-        <v>0.5049118876477245</v>
+        <v>0.5049118878207794</v>
       </c>
       <c r="G44">
-        <v>0.4990974832365696</v>
+        <v>0.4990974832365626</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1415,22 +1415,22 @@
         <v>1.030934397</v>
       </c>
       <c r="B45">
-        <v>1.472937177067241</v>
+        <v>1.472937177743613</v>
       </c>
       <c r="C45">
-        <v>1.557197953086015</v>
+        <v>1.5571979530129</v>
       </c>
       <c r="D45">
-        <v>1.588675048883226</v>
+        <v>1.588675048882149</v>
       </c>
       <c r="E45">
         <v>1.586425072703685</v>
       </c>
       <c r="F45">
-        <v>1.566868158499932</v>
+        <v>1.566868159006285</v>
       </c>
       <c r="G45">
-        <v>1.551243771826023</v>
+        <v>1.551243771826003</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1438,22 +1438,22 @@
         <v>1.479112841</v>
       </c>
       <c r="B46">
-        <v>1.962117043891545</v>
+        <v>1.962117044607471</v>
       </c>
       <c r="C46">
-        <v>2.022817779366698</v>
+        <v>2.02281777939433</v>
       </c>
       <c r="D46">
-        <v>2.089766855834029</v>
+        <v>2.08976685583256</v>
       </c>
       <c r="E46">
         <v>2.087068501116107</v>
       </c>
       <c r="F46">
-        <v>2.048490943802521</v>
+        <v>2.048490944459196</v>
       </c>
       <c r="G46">
-        <v>2.027972967651872</v>
+        <v>2.027972967651845</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1461,22 +1461,22 @@
         <v>1.817472853</v>
       </c>
       <c r="B47">
-        <v>2.269973699151978</v>
+        <v>2.269973697488466</v>
       </c>
       <c r="C47">
-        <v>2.277103438017257</v>
+        <v>2.277103438043807</v>
       </c>
       <c r="D47">
-        <v>2.339561150244085</v>
+        <v>2.339561150242502</v>
       </c>
       <c r="E47">
-        <v>2.33631494824774</v>
+        <v>2.336314948247741</v>
       </c>
       <c r="F47">
-        <v>2.304864302552454</v>
+        <v>2.304864303290234</v>
       </c>
       <c r="G47">
-        <v>2.282422043352566</v>
+        <v>2.282422043352537</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1484,22 +1484,22 @@
         <v>0.369717394</v>
       </c>
       <c r="B48">
-        <v>0.7936619024478585</v>
+        <v>0.7936619029909401</v>
       </c>
       <c r="C48">
-        <v>0.8246021676880634</v>
+        <v>0.8246021676002975</v>
       </c>
       <c r="D48">
-        <v>0.8430871754166407</v>
+        <v>0.8430871754160236</v>
       </c>
       <c r="E48">
-        <v>0.840703016865294</v>
+        <v>0.8407030168652943</v>
       </c>
       <c r="F48">
-        <v>0.8242501689086309</v>
+        <v>0.8242501691819413</v>
       </c>
       <c r="G48">
-        <v>0.8163091628434149</v>
+        <v>0.816309162843404</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1507,22 +1507,22 @@
         <v>-0.162350195</v>
       </c>
       <c r="B49">
-        <v>-0.0797900856147955</v>
+        <v>-0.07979008564074222</v>
       </c>
       <c r="C49">
-        <v>-0.1196113210421587</v>
+        <v>-0.1196113210778009</v>
       </c>
       <c r="D49">
-        <v>-0.09012291515890844</v>
+        <v>-0.09012291515904616</v>
       </c>
       <c r="E49">
-        <v>-0.07954611025494474</v>
+        <v>-0.07954611025494485</v>
       </c>
       <c r="F49">
-        <v>-0.1218664407961437</v>
+        <v>-0.1218664408219997</v>
       </c>
       <c r="G49">
-        <v>-0.1234465852809985</v>
+        <v>-0.1234465852809974</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1530,22 +1530,22 @@
         <v>-0.729825744</v>
       </c>
       <c r="B50">
-        <v>-0.8392456262292167</v>
+        <v>-0.8392456283653114</v>
       </c>
       <c r="C50">
-        <v>-0.9340820165907101</v>
+        <v>-0.9340820165572218</v>
       </c>
       <c r="D50">
-        <v>-0.9040636818637591</v>
+        <v>-0.904063681863421</v>
       </c>
       <c r="E50">
-        <v>-0.9032453343075892</v>
+        <v>-0.9032453343075896</v>
       </c>
       <c r="F50">
-        <v>-0.9357186708482056</v>
+        <v>-0.9357186711316287</v>
       </c>
       <c r="G50">
-        <v>-0.9315286757188939</v>
+        <v>-0.9315286757188824</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1553,22 +1553,22 @@
         <v>-0.317430882</v>
       </c>
       <c r="B51">
-        <v>-0.7801388745152308</v>
+        <v>-0.7801388757159254</v>
       </c>
       <c r="C51">
-        <v>-0.840945717701659</v>
+        <v>-0.8409457176747623</v>
       </c>
       <c r="D51">
-        <v>-0.8174065601517676</v>
+        <v>-0.817406560151447</v>
       </c>
       <c r="E51">
-        <v>-0.8159970336080953</v>
+        <v>-0.8159970336080955</v>
       </c>
       <c r="F51">
-        <v>-0.8429537951184877</v>
+        <v>-0.842953795373012</v>
       </c>
       <c r="G51">
-        <v>-0.8389860725881475</v>
+        <v>-0.8389860725881373</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1576,22 +1576,22 @@
         <v>-0.490640104</v>
       </c>
       <c r="B52">
-        <v>-0.6890392843527992</v>
+        <v>-0.689039284000471</v>
       </c>
       <c r="C52">
-        <v>-0.7046779807708489</v>
+        <v>-0.7046779807546086</v>
       </c>
       <c r="D52">
-        <v>-0.6846239450983359</v>
+        <v>-0.6846239450980729</v>
       </c>
       <c r="E52">
-        <v>-0.682356075445532</v>
+        <v>-0.6823560754455323</v>
       </c>
       <c r="F52">
-        <v>-0.7067700193742028</v>
+        <v>-0.7067700195871465</v>
       </c>
       <c r="G52">
-        <v>-0.7036950152242268</v>
+        <v>-0.7036950152242181</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1599,22 +1599,22 @@
         <v>-1.100609032</v>
       </c>
       <c r="B53">
-        <v>-0.9916440898248269</v>
+        <v>-0.9916440899478505</v>
       </c>
       <c r="C53">
-        <v>-0.985528994060861</v>
+        <v>-0.9855289939775276</v>
       </c>
       <c r="D53">
-        <v>-1.001032703825447</v>
+        <v>-1.001032703824808</v>
       </c>
       <c r="E53">
         <v>-1.000253627624798</v>
       </c>
       <c r="F53">
-        <v>-0.9867710920743045</v>
+        <v>-0.9867710923713263</v>
       </c>
       <c r="G53">
-        <v>-0.9777825800432083</v>
+        <v>-0.9777825800431964</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1622,22 +1622,22 @@
         <v>-0.351083172</v>
       </c>
       <c r="B54">
-        <v>-0.2309549446113124</v>
+        <v>-0.2309549445506254</v>
       </c>
       <c r="C54">
-        <v>-0.2479094776159023</v>
+        <v>-0.2479094776412257</v>
       </c>
       <c r="D54">
-        <v>-0.2375957106565301</v>
+        <v>-0.2375957106564875</v>
       </c>
       <c r="E54">
-        <v>-0.2300768751420275</v>
+        <v>-0.2300768751420276</v>
       </c>
       <c r="F54">
-        <v>-0.2510954253898861</v>
+        <v>-0.2510954254564975</v>
       </c>
       <c r="G54">
-        <v>-0.2507989467217545</v>
+        <v>-0.2507989467217517</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1645,22 +1645,22 @@
         <v>0.476992209</v>
       </c>
       <c r="B55">
-        <v>0.8381025460529791</v>
+        <v>0.8381025466593807</v>
       </c>
       <c r="C55">
-        <v>0.8558953435017539</v>
+        <v>0.855895343430586</v>
       </c>
       <c r="D55">
-        <v>0.8942094393444334</v>
+        <v>0.8942094393436996</v>
       </c>
       <c r="E55">
         <v>0.8909487372470282</v>
       </c>
       <c r="F55">
-        <v>0.857592841933803</v>
+        <v>0.8575928422175573</v>
       </c>
       <c r="G55">
-        <v>0.8493834402192225</v>
+        <v>0.8493834402192112</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1668,22 +1668,22 @@
         <v>1.269210822</v>
       </c>
       <c r="B56">
-        <v>1.516892656278792</v>
+        <v>1.516892656630009</v>
       </c>
       <c r="C56">
-        <v>1.581149966913648</v>
+        <v>1.581149966837677</v>
       </c>
       <c r="D56">
-        <v>1.618554980233333</v>
+        <v>1.618554980232208</v>
       </c>
       <c r="E56">
         <v>1.615355375938674</v>
       </c>
       <c r="F56">
-        <v>1.590061245086363</v>
+        <v>1.590061245600913</v>
       </c>
       <c r="G56">
-        <v>1.574922717260385</v>
+        <v>1.574922717260364</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1691,22 +1691,22 @@
         <v>1.68335771</v>
       </c>
       <c r="B57">
-        <v>1.752196266699112</v>
+        <v>1.752196266474676</v>
       </c>
       <c r="C57">
-        <v>1.779347353817445</v>
+        <v>1.779347353792924</v>
       </c>
       <c r="D57">
-        <v>1.836066513997792</v>
+        <v>1.836066513996483</v>
       </c>
       <c r="E57">
         <v>1.83262180919492</v>
       </c>
       <c r="F57">
-        <v>1.795965198759272</v>
+        <v>1.795965199337737</v>
       </c>
       <c r="G57">
-        <v>1.77874968803559</v>
+        <v>1.778749688035567</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1714,22 +1714,22 @@
         <v>1.248614285</v>
       </c>
       <c r="B58">
-        <v>1.289715001715688</v>
+        <v>1.289715001335042</v>
       </c>
       <c r="C58">
-        <v>1.317314759801752</v>
+        <v>1.31731475970882</v>
       </c>
       <c r="D58">
-        <v>1.334354467822273</v>
+        <v>1.334354467821395</v>
       </c>
       <c r="E58">
         <v>1.332138030516446</v>
       </c>
       <c r="F58">
-        <v>1.321763445176735</v>
+        <v>1.321763445606126</v>
       </c>
       <c r="G58">
-        <v>1.309013353596595</v>
+        <v>1.309013353596577</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1737,22 +1737,22 @@
         <v>0.747520063</v>
       </c>
       <c r="B59">
-        <v>0.6742730435079063</v>
+        <v>0.6742730445647642</v>
       </c>
       <c r="C59">
-        <v>0.7153969205609528</v>
+        <v>0.7153969204902284</v>
       </c>
       <c r="D59">
-        <v>0.7412501308635068</v>
+        <v>0.7412501308629188</v>
       </c>
       <c r="E59">
-        <v>0.7398752307560723</v>
+        <v>0.7398752307560722</v>
       </c>
       <c r="F59">
-        <v>0.7166668485848916</v>
+        <v>0.7166668488232818</v>
       </c>
       <c r="G59">
-        <v>0.7087772430700111</v>
+        <v>0.7087772430700017</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1760,22 +1760,22 @@
         <v>-0.631971431</v>
       </c>
       <c r="B60">
-        <v>-0.4451684893076283</v>
+        <v>-0.4451684906212131</v>
       </c>
       <c r="C60">
-        <v>-0.4820944398376792</v>
+        <v>-0.4820944398350928</v>
       </c>
       <c r="D60">
-        <v>-0.4740257692460477</v>
+        <v>-0.4740257692458545</v>
       </c>
       <c r="E60">
         <v>-0.4735424990365346</v>
       </c>
       <c r="F60">
-        <v>-0.4835780987358104</v>
+        <v>-0.4835780988744101</v>
       </c>
       <c r="G60">
-        <v>-0.4822972224904613</v>
+        <v>-0.4822972224904558</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1783,22 +1783,22 @@
         <v>-0.10813702</v>
       </c>
       <c r="B61">
-        <v>0.1542563161040187</v>
+        <v>0.1542563164794359</v>
       </c>
       <c r="C61">
-        <v>0.1759877441502712</v>
+        <v>0.1759877440878156</v>
       </c>
       <c r="D61">
-        <v>0.1741275484799055</v>
+        <v>0.1741275484797648</v>
       </c>
       <c r="E61">
         <v>0.1735873685934775</v>
       </c>
       <c r="F61">
-        <v>0.1722305111422174</v>
+        <v>0.17223051120973</v>
       </c>
       <c r="G61">
-        <v>0.1696521777234079</v>
+        <v>0.1696521777234053</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1806,22 +1806,22 @@
         <v>0.399434913</v>
       </c>
       <c r="B62">
-        <v>0.6451773731673225</v>
+        <v>0.6451773733723996</v>
       </c>
       <c r="C62">
-        <v>0.6791860627306412</v>
+        <v>0.6791860626267677</v>
       </c>
       <c r="D62">
-        <v>0.6692729622796627</v>
+        <v>0.6692729622792705</v>
       </c>
       <c r="E62">
-        <v>0.6677100176610808</v>
+        <v>0.6677100176610811</v>
       </c>
       <c r="F62">
-        <v>0.6749425683031185</v>
+        <v>0.6749425685300687</v>
       </c>
       <c r="G62">
-        <v>0.6690401321895725</v>
+        <v>0.6690401321895635</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1829,22 +1829,22 @@
         <v>0.598079881</v>
       </c>
       <c r="B63">
-        <v>0.8046347813008677</v>
+        <v>0.8046347817200119</v>
       </c>
       <c r="C63">
-        <v>0.8870830149827136</v>
+        <v>0.8870830148466634</v>
       </c>
       <c r="D63">
-        <v>0.8521195437022739</v>
+        <v>0.8521195437018885</v>
       </c>
       <c r="E63">
-        <v>0.851547951000559</v>
+        <v>0.8515479510005592</v>
       </c>
       <c r="F63">
-        <v>0.8825433157418454</v>
+        <v>0.8825433160343366</v>
       </c>
       <c r="G63">
-        <v>0.8737775699229189</v>
+        <v>0.8737775699229072</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1852,22 +1852,22 @@
         <v>-0.364643642</v>
       </c>
       <c r="B64">
-        <v>-0.1509111654866287</v>
+        <v>-0.1509111654828283</v>
       </c>
       <c r="C64">
-        <v>-0.124723392400293</v>
+        <v>-0.1247233924092499</v>
       </c>
       <c r="D64">
-        <v>-0.1484772770736431</v>
+        <v>-0.1484772770734795</v>
       </c>
       <c r="E64">
-        <v>-0.1481623815579372</v>
+        <v>-0.148162381557937</v>
       </c>
       <c r="F64">
-        <v>-0.1255883765666531</v>
+        <v>-0.1255883765899089</v>
       </c>
       <c r="G64">
-        <v>-0.1257476417013957</v>
+        <v>-0.125747641701395</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -1875,22 +1875,22 @@
         <v>2.015990384</v>
       </c>
       <c r="B65">
-        <v>1.676061455924105</v>
+        <v>1.676061457123847</v>
       </c>
       <c r="C65">
-        <v>1.825354429680765</v>
+        <v>1.825354429608222</v>
       </c>
       <c r="D65">
-        <v>1.856629404641705</v>
+        <v>1.856629404640485</v>
       </c>
       <c r="E65">
         <v>1.854286712336691</v>
       </c>
       <c r="F65">
-        <v>1.838084372459854</v>
+        <v>1.838084373051688</v>
       </c>
       <c r="G65">
-        <v>1.819752804076559</v>
+        <v>1.819752804076536</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -1898,22 +1898,22 @@
         <v>2.364869298</v>
       </c>
       <c r="B66">
-        <v>1.74351392174986</v>
+        <v>1.743513923175322</v>
       </c>
       <c r="C66">
-        <v>1.900760409660915</v>
+        <v>1.900760409604738</v>
       </c>
       <c r="D66">
-        <v>1.939276325967951</v>
+        <v>1.939276325966659</v>
       </c>
       <c r="E66">
         <v>1.936835026170056</v>
       </c>
       <c r="F66">
-        <v>1.916100869740598</v>
+        <v>1.916100870356827</v>
       </c>
       <c r="G66">
-        <v>1.896963291773284</v>
+        <v>1.896963291773259</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -1921,22 +1921,22 @@
         <v>2.827580557</v>
       </c>
       <c r="B67">
-        <v>1.9484892351045</v>
+        <v>1.94848923584483</v>
       </c>
       <c r="C67">
-        <v>2.106841398437367</v>
+        <v>2.106841398333119</v>
       </c>
       <c r="D67">
-        <v>2.118018559531476</v>
+        <v>2.118018559530195</v>
       </c>
       <c r="E67">
         <v>2.115657583434459</v>
       </c>
       <c r="F67">
-        <v>2.119046567075669</v>
+        <v>2.119046567756093</v>
       </c>
       <c r="G67">
-        <v>2.098209076809897</v>
+        <v>2.09820907680987</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -1944,22 +1944,22 @@
         <v>0.626809444</v>
       </c>
       <c r="B68">
-        <v>0.4416979991333775</v>
+        <v>0.4416979992316076</v>
       </c>
       <c r="C68">
-        <v>0.4655231902359929</v>
+        <v>0.4655231901455906</v>
       </c>
       <c r="D68">
-        <v>0.4517003655391711</v>
+        <v>0.4517003655389202</v>
       </c>
       <c r="E68">
-        <v>0.4495670973341337</v>
+        <v>0.449567097334134</v>
       </c>
       <c r="F68">
-        <v>0.4604046194934479</v>
+        <v>0.4604046196543595</v>
       </c>
       <c r="G68">
-        <v>0.4565660743498361</v>
+        <v>0.4565660743498295</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -1967,22 +1967,22 @@
         <v>0.49739888</v>
       </c>
       <c r="B69">
-        <v>0.357203788536871</v>
+        <v>0.3572037886499202</v>
       </c>
       <c r="C69">
-        <v>0.3872810531412412</v>
+        <v>0.3872810530568308</v>
       </c>
       <c r="D69">
-        <v>0.3545279425424572</v>
+        <v>0.3545279425423556</v>
       </c>
       <c r="E69">
-        <v>0.3600913955277237</v>
+        <v>0.360091395527724</v>
       </c>
       <c r="F69">
-        <v>0.3817891552405832</v>
+        <v>0.3817891553766893</v>
       </c>
       <c r="G69">
-        <v>0.3788691845406778</v>
+        <v>0.3788691845406723</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -1990,22 +1990,22 @@
         <v>0.325808278</v>
       </c>
       <c r="B70">
-        <v>-0.01045030165755298</v>
+        <v>-0.01045030139700145</v>
       </c>
       <c r="C70">
-        <v>0.01489432951538064</v>
+        <v>0.01489432947952843</v>
       </c>
       <c r="D70">
-        <v>-0.03015701303982705</v>
+        <v>-0.030157013039634</v>
       </c>
       <c r="E70">
-        <v>-0.03210825128680388</v>
+        <v>-0.03210825128680372</v>
       </c>
       <c r="F70">
-        <v>0.01153541865300601</v>
+        <v>0.01153541867202658</v>
       </c>
       <c r="G70">
-        <v>0.01118800888669403</v>
+        <v>0.01118800888669317</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2013,22 +2013,22 @@
         <v>0.365489314</v>
       </c>
       <c r="B71">
-        <v>0.03554397882882643</v>
+        <v>0.03554397932472505</v>
       </c>
       <c r="C71">
-        <v>0.09649987841310939</v>
+        <v>0.09649987835522517</v>
       </c>
       <c r="D71">
-        <v>0.04953965919805981</v>
+        <v>0.04953965919820952</v>
       </c>
       <c r="E71">
-        <v>0.05428528118395649</v>
+        <v>0.05428528118395663</v>
       </c>
       <c r="F71">
-        <v>0.09276095686987204</v>
+        <v>0.09276095691311487</v>
       </c>
       <c r="G71">
-        <v>0.09056100580139403</v>
+        <v>0.09056100580139229</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2036,22 +2036,22 @@
         <v>1.026844468</v>
       </c>
       <c r="B72">
-        <v>0.6273818095856589</v>
+        <v>0.6273818103432567</v>
       </c>
       <c r="C72">
-        <v>0.7054266905505631</v>
+        <v>0.7054266904476194</v>
       </c>
       <c r="D72">
-        <v>0.6939088747629507</v>
+        <v>0.6939088747625554</v>
       </c>
       <c r="E72">
-        <v>0.6936863903065884</v>
+        <v>0.6936863903065885</v>
       </c>
       <c r="F72">
-        <v>0.7032786906634539</v>
+        <v>0.7032786908978439</v>
       </c>
       <c r="G72">
-        <v>0.6954052015705303</v>
+        <v>0.6954052015705211</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2059,22 +2059,22 @@
         <v>0.699083059</v>
       </c>
       <c r="B73">
-        <v>0.5490537638535454</v>
+        <v>0.5490537669410885</v>
       </c>
       <c r="C73">
-        <v>0.6068633873475181</v>
+        <v>0.6068633873298898</v>
       </c>
       <c r="D73">
-        <v>0.6691945287468452</v>
+        <v>0.6691945287461464</v>
       </c>
       <c r="E73">
-        <v>0.6684072166603916</v>
+        <v>0.6684072166603915</v>
       </c>
       <c r="F73">
-        <v>0.613696457035366</v>
+        <v>0.6136964572397244</v>
       </c>
       <c r="G73">
-        <v>0.6057118133853706</v>
+        <v>0.6057118133853626</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2082,22 +2082,22 @@
         <v>0.662278742</v>
       </c>
       <c r="B74">
-        <v>0.5709598241057691</v>
+        <v>0.5709598268950711</v>
       </c>
       <c r="C74">
-        <v>0.6315903450116488</v>
+        <v>0.6315903449738371</v>
       </c>
       <c r="D74">
-        <v>0.6910484366990367</v>
+        <v>0.6910484366983278</v>
       </c>
       <c r="E74">
         <v>0.6895971279517825</v>
       </c>
       <c r="F74">
-        <v>0.6360395120366503</v>
+        <v>0.6360395122491987</v>
       </c>
       <c r="G74">
-        <v>0.6283433650197858</v>
+        <v>0.6283433650197774</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2105,22 +2105,22 @@
         <v>0.456505507</v>
       </c>
       <c r="B75">
-        <v>0.3184086800024766</v>
+        <v>0.3184086813803343</v>
       </c>
       <c r="C75">
-        <v>0.3331876308491811</v>
+        <v>0.3331876308010954</v>
       </c>
       <c r="D75">
-        <v>0.373768827192924</v>
+        <v>0.3737688271924748</v>
       </c>
       <c r="E75">
-        <v>0.3724055042265779</v>
+        <v>0.3724055042265778</v>
       </c>
       <c r="F75">
-        <v>0.3332176104063387</v>
+        <v>0.3332176105236787</v>
       </c>
       <c r="G75">
-        <v>0.3285343872396828</v>
+        <v>0.3285343872396782</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2128,22 +2128,22 @@
         <v>-0.181605646</v>
       </c>
       <c r="B76">
-        <v>-0.1848648975017363</v>
+        <v>-0.1848648973891894</v>
       </c>
       <c r="C76">
-        <v>-0.1694172321893314</v>
+        <v>-0.1694172321821299</v>
       </c>
       <c r="D76">
-        <v>-0.2166328660306682</v>
+        <v>-0.2166328660303428</v>
       </c>
       <c r="E76">
-        <v>-0.2204779539717663</v>
+        <v>-0.2204779539717662</v>
       </c>
       <c r="F76">
-        <v>-0.1722907951295035</v>
+        <v>-0.1722907951667788</v>
       </c>
       <c r="G76">
-        <v>-0.1687903262635255</v>
+        <v>-0.1687903262635242</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2151,22 +2151,22 @@
         <v>0.647849754</v>
       </c>
       <c r="B77">
-        <v>0.421507952045728</v>
+        <v>0.4215079526921449</v>
       </c>
       <c r="C77">
-        <v>0.4307521608290664</v>
+        <v>0.4307521607645295</v>
       </c>
       <c r="D77">
-        <v>0.4560940523205986</v>
+        <v>0.4560940523201704</v>
       </c>
       <c r="E77">
-        <v>0.4539615008875778</v>
+        <v>0.4539615008875777</v>
       </c>
       <c r="F77">
-        <v>0.4292307810853788</v>
+        <v>0.4292307812336733</v>
       </c>
       <c r="G77">
-        <v>0.4244744196656008</v>
+        <v>0.424474419665595</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2174,22 +2174,22 @@
         <v>-0.151031448</v>
       </c>
       <c r="B78">
-        <v>-0.4414734803028272</v>
+        <v>-0.4414734802421283</v>
       </c>
       <c r="C78">
-        <v>-0.4478381464305867</v>
+        <v>-0.4478381464343915</v>
       </c>
       <c r="D78">
-        <v>-0.4402231794755744</v>
+        <v>-0.4402231794753995</v>
       </c>
       <c r="E78">
         <v>-0.4417083675761468</v>
       </c>
       <c r="F78">
-        <v>-0.4415890530977059</v>
+        <v>-0.4415890532265882</v>
       </c>
       <c r="G78">
-        <v>-0.4486778761222873</v>
+        <v>-0.4486778761222822</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2197,22 +2197,22 @@
         <v>0.204622557</v>
       </c>
       <c r="B79">
-        <v>-0.03954956870725881</v>
+        <v>-0.03954956793619075</v>
       </c>
       <c r="C79">
-        <v>-0.01579833822757189</v>
+        <v>-0.01579833827254072</v>
       </c>
       <c r="D79">
-        <v>0.001458433699444504</v>
+        <v>0.001458433699311923</v>
       </c>
       <c r="E79">
-        <v>0.0009536075454882123</v>
+        <v>0.0009536075454881533</v>
       </c>
       <c r="F79">
-        <v>-0.01887096345199436</v>
+        <v>-0.01887096344476689</v>
       </c>
       <c r="G79">
-        <v>-0.02050156642427816</v>
+        <v>-0.02050156642427843</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2220,22 +2220,22 @@
         <v>0.6727765610000001</v>
       </c>
       <c r="B80">
-        <v>0.556046444594037</v>
+        <v>0.5560464449135224</v>
       </c>
       <c r="C80">
-        <v>0.6183756759792974</v>
+        <v>0.6183756758666743</v>
       </c>
       <c r="D80">
-        <v>0.5769013195781117</v>
+        <v>0.5769013195779183</v>
       </c>
       <c r="E80">
-        <v>0.576946526251128</v>
+        <v>0.5769465262511282</v>
       </c>
       <c r="F80">
-        <v>0.6133098558641772</v>
+        <v>0.6133098560726664</v>
       </c>
       <c r="G80">
-        <v>0.6072452856613115</v>
+        <v>0.6072452856613031</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2243,22 +2243,22 @@
         <v>1.409854459</v>
       </c>
       <c r="B81">
-        <v>1.238648359004779</v>
+        <v>1.23864835846565</v>
       </c>
       <c r="C81">
-        <v>1.30945907792439</v>
+        <v>1.309459077751803</v>
       </c>
       <c r="D81">
-        <v>1.268139749407778</v>
+        <v>1.268139749407179</v>
       </c>
       <c r="E81">
         <v>1.266854557429598</v>
       </c>
       <c r="F81">
-        <v>1.304941081216051</v>
+        <v>1.304941081642034</v>
       </c>
       <c r="G81">
-        <v>1.292768254126317</v>
+        <v>1.2927682541263</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2266,22 +2266,22 @@
         <v>1.436857019</v>
       </c>
       <c r="B82">
-        <v>1.189181056513954</v>
+        <v>1.189181054470793</v>
       </c>
       <c r="C82">
-        <v>1.220420741464306</v>
+        <v>1.220420741266864</v>
       </c>
       <c r="D82">
-        <v>1.14632244738794</v>
+        <v>1.146322447387556</v>
       </c>
       <c r="E82">
         <v>1.146644075181984</v>
       </c>
       <c r="F82">
-        <v>1.211889610336847</v>
+        <v>1.21188961073329</v>
       </c>
       <c r="G82">
-        <v>1.201015595770325</v>
+        <v>1.201015595770309</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2289,22 +2289,22 @@
         <v>-0.078187413</v>
       </c>
       <c r="B83">
-        <v>-0.4777878543076751</v>
+        <v>-0.4777878517646848</v>
       </c>
       <c r="C83">
-        <v>-0.3937493333717514</v>
+        <v>-0.3937493332930366</v>
       </c>
       <c r="D83">
-        <v>-0.4551802763631115</v>
+        <v>-0.4551802763625509</v>
       </c>
       <c r="E83">
-        <v>-0.4298146990220087</v>
+        <v>-0.4298146990220084</v>
       </c>
       <c r="F83">
-        <v>-0.3731231703174516</v>
+        <v>-0.3731231704237526</v>
       </c>
       <c r="G83">
-        <v>-0.3858372622832796</v>
+        <v>-0.3858372622832756</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2312,22 +2312,22 @@
         <v>-0.089819775</v>
       </c>
       <c r="B84">
-        <v>-0.3142111558404572</v>
+        <v>-0.3142111532803021</v>
       </c>
       <c r="C84">
-        <v>-0.2037499776629884</v>
+        <v>-0.2037499776339326</v>
       </c>
       <c r="D84">
-        <v>-0.2730224857996708</v>
+        <v>-0.2730224857991948</v>
       </c>
       <c r="E84">
-        <v>-0.2670738637401383</v>
+        <v>-0.267073863740138</v>
       </c>
       <c r="F84">
-        <v>-0.1997308234811588</v>
+        <v>-0.1997308235287824</v>
       </c>
       <c r="G84">
-        <v>-0.2008598702266254</v>
+        <v>-0.2008598702266237</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2335,22 +2335,22 @@
         <v>-0.951749297</v>
       </c>
       <c r="B85">
-        <v>-1.052109686561751</v>
+        <v>-1.052109682200372</v>
       </c>
       <c r="C85">
-        <v>-0.9116751298280076</v>
+        <v>-0.9116751296343498</v>
       </c>
       <c r="D85">
-        <v>-0.9689286909449275</v>
+        <v>-0.9689286909440492</v>
       </c>
       <c r="E85">
-        <v>-0.9560024607358224</v>
+        <v>-0.9560024607358223</v>
       </c>
       <c r="F85">
-        <v>-0.8910776379561405</v>
+        <v>-0.8910776382232894</v>
       </c>
       <c r="G85">
-        <v>-0.892228001272906</v>
+        <v>-0.8922280012728956</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2358,22 +2358,22 @@
         <v>-0.611776729</v>
       </c>
       <c r="B86">
-        <v>-0.5152780790701409</v>
+        <v>-0.5152780755148332</v>
       </c>
       <c r="C86">
-        <v>-0.379342278324024</v>
+        <v>-0.379342278268806</v>
       </c>
       <c r="D86">
-        <v>-0.4344840166021993</v>
+        <v>-0.4344840166016919</v>
       </c>
       <c r="E86">
-        <v>-0.4307347783553209</v>
+        <v>-0.4307347783553207</v>
       </c>
       <c r="F86">
-        <v>-0.3747944484144171</v>
+        <v>-0.3747944485169569</v>
       </c>
       <c r="G86">
-        <v>-0.3738892762197565</v>
+        <v>-0.3738892762197526</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2381,22 +2381,22 @@
         <v>-1.503113365</v>
       </c>
       <c r="B87">
-        <v>-1.586393339327478</v>
+        <v>-1.586393333853157</v>
       </c>
       <c r="C87">
-        <v>-1.48370240887223</v>
+        <v>-1.483702408555807</v>
       </c>
       <c r="D87">
-        <v>-1.49359982002898</v>
+        <v>-1.493599820027991</v>
       </c>
       <c r="E87">
-        <v>-1.472931567305363</v>
+        <v>-1.472931567305362</v>
       </c>
       <c r="F87">
-        <v>-1.43441215995543</v>
+        <v>-1.434412160399382</v>
       </c>
       <c r="G87">
-        <v>-1.451950752863</v>
+        <v>-1.451950752862983</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2404,22 +2404,22 @@
         <v>-0.95035541</v>
       </c>
       <c r="B88">
-        <v>-1.359712421820794</v>
+        <v>-1.359712416482687</v>
       </c>
       <c r="C88">
-        <v>-1.270249079690172</v>
+        <v>-1.270249079454969</v>
       </c>
       <c r="D88">
-        <v>-1.262364017559159</v>
+        <v>-1.262364017558427</v>
       </c>
       <c r="E88">
         <v>-1.258136751307304</v>
       </c>
       <c r="F88">
-        <v>-1.247702933144301</v>
+        <v>-1.247702933521181</v>
       </c>
       <c r="G88">
-        <v>-1.246812125971369</v>
+        <v>-1.246812125971354</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2427,22 +2427,22 @@
         <v>-0.869041164</v>
       </c>
       <c r="B89">
-        <v>-0.7851434816221632</v>
+        <v>-0.7851434786380161</v>
       </c>
       <c r="C89">
-        <v>-0.6996496378221233</v>
+        <v>-0.6996496377077648</v>
       </c>
       <c r="D89">
-        <v>-0.7337465210506262</v>
+        <v>-0.7337465210500311</v>
       </c>
       <c r="E89">
-        <v>-0.7233160701090293</v>
+        <v>-0.7233160701090291</v>
       </c>
       <c r="F89">
-        <v>-0.6836549404235243</v>
+        <v>-0.6836549406256648</v>
       </c>
       <c r="G89">
-        <v>-0.6883184398707158</v>
+        <v>-0.6883184398707081</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2450,22 +2450,22 @@
         <v>-0.621619324</v>
       </c>
       <c r="B90">
-        <v>-0.677128589635013</v>
+        <v>-0.6771285866481079</v>
       </c>
       <c r="C90">
-        <v>-0.5897337829816257</v>
+        <v>-0.5897337828728689</v>
       </c>
       <c r="D90">
-        <v>-0.6373983816275157</v>
+        <v>-0.6373983816269089</v>
       </c>
       <c r="E90">
-        <v>-0.5752366095387815</v>
+        <v>-0.5752366095387813</v>
       </c>
       <c r="F90">
-        <v>-0.5316621944983766</v>
+        <v>-0.5316621946674033</v>
       </c>
       <c r="G90">
-        <v>-0.5788725544091173</v>
+        <v>-0.5788725544091109</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2473,22 +2473,22 @@
         <v>0.820733698</v>
       </c>
       <c r="B91">
-        <v>0.285777590627243</v>
+        <v>0.2857775914272223</v>
       </c>
       <c r="C91">
-        <v>0.3597080126874935</v>
+        <v>0.3597080126085314</v>
       </c>
       <c r="D91">
-        <v>0.2918760664522472</v>
+        <v>0.2918760664523546</v>
       </c>
       <c r="E91">
-        <v>0.2946733277608243</v>
+        <v>0.2946733277608246</v>
       </c>
       <c r="F91">
-        <v>0.3559721694754757</v>
+        <v>0.3559721696032044</v>
       </c>
       <c r="G91">
-        <v>0.3518402864698799</v>
+        <v>0.3518402864698747</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2496,22 +2496,22 @@
         <v>1.157975086</v>
       </c>
       <c r="B92">
-        <v>0.6004952846713671</v>
+        <v>0.6004952847976842</v>
       </c>
       <c r="C92">
-        <v>0.6605940569911345</v>
+        <v>0.6605940568690289</v>
       </c>
       <c r="D92">
-        <v>0.579085994258474</v>
+        <v>0.5790859942584703</v>
       </c>
       <c r="E92">
-        <v>0.5815131868453562</v>
+        <v>0.5815131868453566</v>
       </c>
       <c r="F92">
-        <v>0.6546266267354148</v>
+        <v>0.6546266269577329</v>
       </c>
       <c r="G92">
-        <v>0.6485131042536084</v>
+        <v>0.6485131042535994</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2519,22 +2519,22 @@
         <v>1.16180901</v>
       </c>
       <c r="B93">
-        <v>0.6294734125725581</v>
+        <v>0.629473412497797</v>
       </c>
       <c r="C93">
-        <v>0.6905522250674461</v>
+        <v>0.6905522249364631</v>
       </c>
       <c r="D93">
-        <v>0.6045694025600044</v>
+        <v>0.6045694025600047</v>
       </c>
       <c r="E93">
-        <v>0.6070933944593444</v>
+        <v>0.6070933944593447</v>
       </c>
       <c r="F93">
-        <v>0.6839090799293209</v>
+        <v>0.6839090801606325</v>
       </c>
       <c r="G93">
-        <v>0.6775688252225025</v>
+        <v>0.6775688252224931</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2542,22 +2542,22 @@
         <v>0.673844651</v>
       </c>
       <c r="B94">
-        <v>0.3754932510357367</v>
+        <v>0.3754932513998903</v>
       </c>
       <c r="C94">
-        <v>0.4388537507077194</v>
+        <v>0.4388537506141158</v>
       </c>
       <c r="D94">
-        <v>0.3679879864136181</v>
+        <v>0.3679879864136921</v>
       </c>
       <c r="E94">
-        <v>0.3716528245945575</v>
+        <v>0.3716528245945577</v>
       </c>
       <c r="F94">
-        <v>0.4340509325314558</v>
+        <v>0.4340509326837016</v>
       </c>
       <c r="G94">
-        <v>0.4295305223754124</v>
+        <v>0.4295305223754062</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2565,22 +2565,22 @@
         <v>0.576154411</v>
       </c>
       <c r="B95">
-        <v>0.1903608941954839</v>
+        <v>0.1903608953149541</v>
       </c>
       <c r="C95">
-        <v>0.2715405943752677</v>
+        <v>0.2715405943125805</v>
       </c>
       <c r="D95">
-        <v>0.1996166016695815</v>
+        <v>0.1996166016697674</v>
       </c>
       <c r="E95">
-        <v>0.2031224053732677</v>
+        <v>0.203122405373268</v>
       </c>
       <c r="F95">
-        <v>0.2688952582785163</v>
+        <v>0.2688952583788535</v>
       </c>
       <c r="G95">
-        <v>0.2652903133908093</v>
+        <v>0.2652903133908052</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2588,22 +2588,22 @@
         <v>-0.247999935</v>
       </c>
       <c r="B96">
-        <v>-0.4680051100469012</v>
+        <v>-0.4680051071522791</v>
       </c>
       <c r="C96">
-        <v>-0.355882737439576</v>
+        <v>-0.3558827373759933</v>
       </c>
       <c r="D96">
-        <v>-0.4225844268180495</v>
+        <v>-0.4225844268174876</v>
       </c>
       <c r="E96">
-        <v>-0.4147008649077887</v>
+        <v>-0.4147008649077885</v>
       </c>
       <c r="F96">
-        <v>-0.3483573783036656</v>
+        <v>-0.3483573783984094</v>
       </c>
       <c r="G96">
-        <v>-0.3495233878854929</v>
+        <v>-0.3495233878854893</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2611,22 +2611,22 @@
         <v>-1.022406207</v>
       </c>
       <c r="B97">
-        <v>-1.262701318043716</v>
+        <v>-1.262701313287432</v>
       </c>
       <c r="C97">
-        <v>-1.121134306791748</v>
+        <v>-1.121134306539448</v>
       </c>
       <c r="D97">
-        <v>-1.174168600566033</v>
+        <v>-1.174168600565034</v>
       </c>
       <c r="E97">
         <v>-1.150678796070029</v>
       </c>
       <c r="F97">
-        <v>-1.086811412622226</v>
+        <v>-1.086811412954209</v>
       </c>
       <c r="G97">
-        <v>-1.095741797929698</v>
+        <v>-1.095741797929685</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2634,22 +2634,22 @@
         <v>-0.898568511</v>
       </c>
       <c r="B98">
-        <v>-0.9033686897458492</v>
+        <v>-0.9033686851803443</v>
       </c>
       <c r="C98">
-        <v>-0.7586250315993709</v>
+        <v>-0.758625031453422</v>
       </c>
       <c r="D98">
-        <v>-0.8078951553869982</v>
+        <v>-0.8078951553862713</v>
       </c>
       <c r="E98">
-        <v>-0.8016652130355983</v>
+        <v>-0.8016652130355982</v>
       </c>
       <c r="F98">
-        <v>-0.7460759559053234</v>
+        <v>-0.7460759561250787</v>
       </c>
       <c r="G98">
-        <v>-0.7440330483802108</v>
+        <v>-0.7440330483802021</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2657,22 +2657,22 @@
         <v>-0.35746994</v>
       </c>
       <c r="B99">
-        <v>-0.2817707209686929</v>
+        <v>-0.2817707184184445</v>
       </c>
       <c r="C99">
-        <v>-0.1733991372671526</v>
+        <v>-0.1733991372653879</v>
       </c>
       <c r="D99">
-        <v>-0.2144451955592085</v>
+        <v>-0.2144451955589171</v>
       </c>
       <c r="E99">
-        <v>-0.2124353201530395</v>
+        <v>-0.2124353201530393</v>
       </c>
       <c r="F99">
-        <v>-0.1730317151349249</v>
+        <v>-0.1730317151739461</v>
       </c>
       <c r="G99">
-        <v>-0.1733491934187273</v>
+        <v>-0.1733491934187259</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2680,22 +2680,22 @@
         <v>-0.676801503</v>
       </c>
       <c r="B100">
-        <v>-0.03589502887764444</v>
+        <v>-0.03589502664881495</v>
       </c>
       <c r="C100">
-        <v>0.05942264186982299</v>
+        <v>0.05942264183526662</v>
       </c>
       <c r="D100">
-        <v>0.02956448087241769</v>
+        <v>0.02956448087250192</v>
       </c>
       <c r="E100">
-        <v>0.03000339536705278</v>
+        <v>0.03000339536705296</v>
       </c>
       <c r="F100">
-        <v>0.05773666947480755</v>
+        <v>0.05773666950914638</v>
       </c>
       <c r="G100">
-        <v>0.0559038713821802</v>
+        <v>0.05590387138217869</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -2703,22 +2703,22 @@
         <v>-0.963128334</v>
       </c>
       <c r="B101">
-        <v>-0.2714814017398893</v>
+        <v>-0.2714813996923306</v>
       </c>
       <c r="C101">
-        <v>-0.1862343569058221</v>
+        <v>-0.1862343568994309</v>
       </c>
       <c r="D101">
-        <v>-0.2274014537224762</v>
+        <v>-0.2274014537221751</v>
       </c>
       <c r="E101">
-        <v>-0.2242591707024238</v>
+        <v>-0.2242591707024237</v>
       </c>
       <c r="F101">
-        <v>-0.1846713402224348</v>
+        <v>-0.1846713402652682</v>
       </c>
       <c r="G101">
-        <v>-0.1857110303861149</v>
+        <v>-0.1857110303861134</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -2726,22 +2726,22 @@
         <v>-1.089650457</v>
       </c>
       <c r="B102">
-        <v>-0.5433107140660197</v>
+        <v>-0.543310711331521</v>
       </c>
       <c r="C102">
-        <v>-0.4559610482985468</v>
+        <v>-0.4559610482209983</v>
       </c>
       <c r="D102">
-        <v>-0.5055170572928198</v>
+        <v>-0.5055170572922909</v>
       </c>
       <c r="E102">
-        <v>-0.4879341102759703</v>
+        <v>-0.4879341102759701</v>
       </c>
       <c r="F102">
-        <v>-0.4386964006971953</v>
+        <v>-0.4386964008233007</v>
       </c>
       <c r="G102">
-        <v>-0.4482396553469532</v>
+        <v>-0.4482396553469484</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2749,22 +2749,22 @@
         <v>-1.754660522</v>
       </c>
       <c r="B103">
-        <v>-1.119628521979138</v>
+        <v>-1.119628518689733</v>
       </c>
       <c r="C103">
-        <v>-1.043900961810566</v>
+        <v>-1.043900961581805</v>
       </c>
       <c r="D103">
-        <v>-1.089818105778403</v>
+        <v>-1.089818105777498</v>
       </c>
       <c r="E103">
         <v>-1.09553268142206</v>
       </c>
       <c r="F103">
-        <v>-1.036630924370463</v>
+        <v>-1.036630924677298</v>
       </c>
       <c r="G103">
-        <v>-1.020901351224649</v>
+        <v>-1.020901351224637</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -2772,22 +2772,22 @@
         <v>-1.724252511</v>
       </c>
       <c r="B104">
-        <v>-1.679550447394871</v>
+        <v>-1.679550443666403</v>
       </c>
       <c r="C104">
-        <v>-1.617336650811457</v>
+        <v>-1.617336650393944</v>
       </c>
       <c r="D104">
-        <v>-1.656937217936563</v>
+        <v>-1.656937217935285</v>
       </c>
       <c r="E104">
         <v>-1.660293057843189</v>
       </c>
       <c r="F104">
-        <v>-1.59496376744376</v>
+        <v>-1.594963767926163</v>
       </c>
       <c r="G104">
-        <v>-1.575090998950109</v>
+        <v>-1.57509099895009</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -2795,22 +2795,22 @@
         <v>-1.868408762</v>
       </c>
       <c r="B105">
-        <v>-1.900088286530587</v>
+        <v>-1.900088281981663</v>
       </c>
       <c r="C105">
-        <v>-1.850188141357937</v>
+        <v>-1.850188140817828</v>
       </c>
       <c r="D105">
-        <v>-1.885612660699171</v>
+        <v>-1.885612660697728</v>
       </c>
       <c r="E105">
         <v>-1.889241271865125</v>
       </c>
       <c r="F105">
-        <v>-1.818030660693425</v>
+        <v>-1.818030661244866</v>
       </c>
       <c r="G105">
-        <v>-1.795288931054533</v>
+        <v>-1.795288931054512</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2818,22 +2818,22 @@
         <v>-0.07703964000000001</v>
       </c>
       <c r="B106">
-        <v>-0.515716290008461</v>
+        <v>-0.5157162875729899</v>
       </c>
       <c r="C106">
-        <v>-0.4411523900570033</v>
+        <v>-0.4411523899697865</v>
       </c>
       <c r="D106">
-        <v>-0.5000012488317244</v>
+        <v>-0.5000012488311479</v>
       </c>
       <c r="E106">
-        <v>-0.5214960445832146</v>
+        <v>-0.5214960445832144</v>
       </c>
       <c r="F106">
-        <v>-0.4511678313383607</v>
+        <v>-0.4511678314581786</v>
       </c>
       <c r="G106">
-        <v>-0.4323969088358474</v>
+        <v>-0.4323969088358427</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -2841,22 +2841,22 @@
         <v>-0.058419279</v>
       </c>
       <c r="B107">
-        <v>-0.6100463584189995</v>
+        <v>-0.6100463556619444</v>
       </c>
       <c r="C107">
-        <v>-0.52800045452148</v>
+        <v>-0.5280004544099512</v>
       </c>
       <c r="D107">
-        <v>-0.5867356830944427</v>
+        <v>-0.5867356830938075</v>
       </c>
       <c r="E107">
-        <v>-0.444888837640199</v>
+        <v>-0.4448888376401987</v>
       </c>
       <c r="F107">
-        <v>-0.4196810746145643</v>
+        <v>-0.4196810747657454</v>
       </c>
       <c r="G107">
-        <v>-0.5167799696232546</v>
+        <v>-0.5167799696232488</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -2864,22 +2864,22 @@
         <v>1.204247991</v>
       </c>
       <c r="B108">
-        <v>0.6383069974699784</v>
+        <v>0.6383069973262471</v>
       </c>
       <c r="C108">
-        <v>0.7169714648722891</v>
+        <v>0.71697146473115</v>
       </c>
       <c r="D108">
-        <v>0.6370132703028055</v>
+        <v>0.6370132703027548</v>
       </c>
       <c r="E108">
-        <v>0.6384220669926095</v>
+        <v>0.6384220669926098</v>
       </c>
       <c r="F108">
-        <v>0.7099351835629149</v>
+        <v>0.7099351838015669</v>
       </c>
       <c r="G108">
-        <v>0.7029461303229904</v>
+        <v>0.7029461303229808</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2887,22 +2887,22 @@
         <v>1.183657404</v>
       </c>
       <c r="B109">
-        <v>1.271824001370029</v>
+        <v>1.27182399939069</v>
       </c>
       <c r="C109">
-        <v>1.326554891786633</v>
+        <v>1.326554891581208</v>
       </c>
       <c r="D109">
-        <v>1.254257614044028</v>
+        <v>1.254257614043573</v>
       </c>
       <c r="E109">
-        <v>1.254078701580547</v>
+        <v>1.254078701580548</v>
       </c>
       <c r="F109">
-        <v>1.319014199677421</v>
+        <v>1.319014200107225</v>
       </c>
       <c r="G109">
-        <v>1.306424786589047</v>
+        <v>1.306424786589029</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -2910,22 +2910,22 @@
         <v>1.235714724</v>
       </c>
       <c r="B110">
-        <v>1.541249144351359</v>
+        <v>1.541249141671778</v>
       </c>
       <c r="C110">
-        <v>1.581165568574391</v>
+        <v>1.581165568370438</v>
       </c>
       <c r="D110">
-        <v>1.52487967038452</v>
+        <v>1.524879670383841</v>
       </c>
       <c r="E110">
         <v>1.524088770989281</v>
       </c>
       <c r="F110">
-        <v>1.576584355480867</v>
+        <v>1.576584355991212</v>
       </c>
       <c r="G110">
-        <v>1.561466532206067</v>
+        <v>1.561466532206047</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2933,22 +2933,22 @@
         <v>1.193822144</v>
       </c>
       <c r="B111">
-        <v>1.004832013882966</v>
+        <v>1.004832013624319</v>
       </c>
       <c r="C111">
-        <v>1.085424359249898</v>
+        <v>1.085424359096062</v>
       </c>
       <c r="D111">
-        <v>1.046811696727112</v>
+        <v>1.04681169672663</v>
       </c>
       <c r="E111">
         <v>1.046065714959494</v>
       </c>
       <c r="F111">
-        <v>1.081047867336749</v>
+        <v>1.081047867691634</v>
       </c>
       <c r="G111">
-        <v>1.070462357024903</v>
+        <v>1.070462357024889</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -2956,22 +2956,22 @@
         <v>1.680661976</v>
       </c>
       <c r="B112">
-        <v>1.50360797490548</v>
+        <v>1.503607973815888</v>
       </c>
       <c r="C112">
-        <v>1.574261917541133</v>
+        <v>1.574261917368666</v>
       </c>
       <c r="D112">
-        <v>1.545695758522832</v>
+        <v>1.54569575852202</v>
       </c>
       <c r="E112">
         <v>1.543770469612683</v>
       </c>
       <c r="F112">
-        <v>1.57261979204509</v>
+        <v>1.572619792555156</v>
       </c>
       <c r="G112">
-        <v>1.557871753086364</v>
+        <v>1.557871753086343</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -2979,22 +2979,22 @@
         <v>1.735508276</v>
       </c>
       <c r="B113">
-        <v>1.715104650206121</v>
+        <v>1.715104648449981</v>
       </c>
       <c r="C113">
-        <v>1.771628490826369</v>
+        <v>1.771628490657847</v>
       </c>
       <c r="D113">
-        <v>1.749247930264708</v>
+        <v>1.749247930263758</v>
       </c>
       <c r="E113">
-        <v>1.747077229977884</v>
+        <v>1.747077229977885</v>
       </c>
       <c r="F113">
-        <v>1.772506198857605</v>
+        <v>1.772506199430236</v>
       </c>
       <c r="G113">
-        <v>1.755867534524231</v>
+        <v>1.755867534524208</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3002,22 +3002,22 @@
         <v>1.120645867</v>
       </c>
       <c r="B114">
-        <v>1.612899742291628</v>
+        <v>1.612899740362318</v>
       </c>
       <c r="C114">
-        <v>1.669235965131207</v>
+        <v>1.66923596493311</v>
       </c>
       <c r="D114">
-        <v>1.623294584685083</v>
+        <v>1.623294584684302</v>
       </c>
       <c r="E114">
         <v>1.621707627454751</v>
       </c>
       <c r="F114">
-        <v>1.665824474570167</v>
+        <v>1.665824475109505</v>
       </c>
       <c r="G114">
-        <v>1.650250926654348</v>
+        <v>1.650250926654327</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3025,22 +3025,22 @@
         <v>0.220765723</v>
       </c>
       <c r="B115">
-        <v>0.4721540699522533</v>
+        <v>0.4721540703437359</v>
       </c>
       <c r="C115">
-        <v>0.5431417289582396</v>
+        <v>0.5431417288501725</v>
       </c>
       <c r="D115">
-        <v>0.4740264926270095</v>
+        <v>0.4740264926270099</v>
       </c>
       <c r="E115">
-        <v>0.4757995474037909</v>
+        <v>0.4757995474037912</v>
       </c>
       <c r="F115">
-        <v>0.5378167293226019</v>
+        <v>0.5378167295075758</v>
       </c>
       <c r="G115">
-        <v>0.5324096345505995</v>
+        <v>0.532409634550592</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3048,22 +3048,22 @@
         <v>0.291028273</v>
       </c>
       <c r="B116">
-        <v>0.3823678462084131</v>
+        <v>0.382367846848612</v>
       </c>
       <c r="C116">
-        <v>0.4475071810140517</v>
+        <v>0.4475071809273498</v>
       </c>
       <c r="D116">
-        <v>0.3678423104601097</v>
+        <v>0.3678423104602295</v>
       </c>
       <c r="E116">
-        <v>0.3719501329474798</v>
+        <v>0.3719501329474801</v>
       </c>
       <c r="F116">
-        <v>0.4436624774850198</v>
+        <v>0.4436624776408306</v>
       </c>
       <c r="G116">
-        <v>0.4389212364542888</v>
+        <v>0.4389212364542825</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3071,22 +3071,22 @@
         <v>0.583045483</v>
       </c>
       <c r="B117">
-        <v>1.120466298343584</v>
+        <v>1.120466296853424</v>
       </c>
       <c r="C117">
-        <v>1.164538287048211</v>
+        <v>1.164538286849639</v>
       </c>
       <c r="D117">
-        <v>1.077004408047078</v>
+        <v>1.077004408046796</v>
       </c>
       <c r="E117">
         <v>1.077611926340327</v>
       </c>
       <c r="F117">
-        <v>1.155296342755817</v>
+        <v>1.155296343135262</v>
       </c>
       <c r="G117">
-        <v>1.144955285247571</v>
+        <v>1.144955285247555</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3094,22 +3094,22 @@
         <v>1.459657324</v>
       </c>
       <c r="B118">
-        <v>1.522327794833215</v>
+        <v>1.522327791668313</v>
       </c>
       <c r="C118">
-        <v>1.535171145331083</v>
+        <v>1.535171145107328</v>
       </c>
       <c r="D118">
-        <v>1.461668448374352</v>
+        <v>1.461668448373782</v>
       </c>
       <c r="E118">
         <v>1.461385815940258</v>
       </c>
       <c r="F118">
-        <v>1.527190341078343</v>
+        <v>1.527190341573646</v>
       </c>
       <c r="G118">
-        <v>1.513338067323624</v>
+        <v>1.513338067323604</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3117,22 +3117,22 @@
         <v>0.957846139</v>
       </c>
       <c r="B119">
-        <v>1.302945305731832</v>
+        <v>1.302945303299518</v>
       </c>
       <c r="C119">
-        <v>1.337518214282309</v>
+        <v>1.33751821406895</v>
       </c>
       <c r="D119">
-        <v>1.258422139095099</v>
+        <v>1.258422139094671</v>
       </c>
       <c r="E119">
-        <v>1.258493690901554</v>
+        <v>1.258493690901555</v>
       </c>
       <c r="F119">
-        <v>1.328878091666707</v>
+        <v>1.328878092099837</v>
       </c>
       <c r="G119">
-        <v>1.316565082762731</v>
+        <v>1.316565082762714</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3140,22 +3140,22 @@
         <v>1.102629823</v>
       </c>
       <c r="B120">
-        <v>0.4378266474941659</v>
+        <v>0.437826648007514</v>
       </c>
       <c r="C120">
-        <v>0.5260979651039619</v>
+        <v>0.5260979649925716</v>
       </c>
       <c r="D120">
-        <v>0.4476738288746969</v>
+        <v>0.4476738288747563</v>
       </c>
       <c r="E120">
-        <v>0.4496111243239606</v>
+        <v>0.4496111243239609</v>
       </c>
       <c r="F120">
-        <v>0.5204185358528619</v>
+        <v>0.5204185360319896</v>
       </c>
       <c r="G120">
-        <v>0.5149967946893524</v>
+        <v>0.5149967946893451</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3163,22 +3163,22 @@
         <v>1.64061108</v>
       </c>
       <c r="B121">
-        <v>1.401880232773351</v>
+        <v>1.401880230335193</v>
       </c>
       <c r="C121">
-        <v>1.448562831128002</v>
+        <v>1.448562830913245</v>
       </c>
       <c r="D121">
-        <v>1.376973507755409</v>
+        <v>1.376973507754879</v>
       </c>
       <c r="E121">
         <v>1.376600474144181</v>
       </c>
       <c r="F121">
-        <v>1.441297528150739</v>
+        <v>1.441297528618942</v>
       </c>
       <c r="G121">
-        <v>1.427582957659036</v>
+        <v>1.427582957659017</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3186,22 +3186,22 @@
         <v>1.886908677</v>
       </c>
       <c r="B122">
-        <v>1.473087449825604</v>
+        <v>1.473087447377131</v>
       </c>
       <c r="C122">
-        <v>1.517257234819233</v>
+        <v>1.517257234617941</v>
       </c>
       <c r="D122">
-        <v>1.460269506762434</v>
+        <v>1.460269506761795</v>
       </c>
       <c r="E122">
-        <v>1.459563836189338</v>
+        <v>1.459563836189339</v>
       </c>
       <c r="F122">
-        <v>1.512284529838522</v>
+        <v>1.512284530328691</v>
       </c>
       <c r="G122">
-        <v>1.497768789223612</v>
+        <v>1.497768789223592</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3209,22 +3209,22 @@
         <v>1.733513011</v>
       </c>
       <c r="B123">
-        <v>1.826815654868884</v>
+        <v>1.826815652772518</v>
       </c>
       <c r="C123">
-        <v>1.886413112312805</v>
+        <v>1.8864131121447</v>
       </c>
       <c r="D123">
-        <v>1.862104331721683</v>
+        <v>1.862104331720682</v>
       </c>
       <c r="E123">
         <v>1.860255503237003</v>
       </c>
       <c r="F123">
-        <v>1.88897651754321</v>
+        <v>1.888976518151738</v>
       </c>
       <c r="G123">
-        <v>1.870819604390736</v>
+        <v>1.870819604390712</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3232,22 +3232,22 @@
         <v>-0.0362457</v>
       </c>
       <c r="B124">
-        <v>0.3777556690166893</v>
+        <v>0.3777556703659038</v>
       </c>
       <c r="C124">
-        <v>0.4680064951662828</v>
+        <v>0.4680064950747977</v>
       </c>
       <c r="D124">
-        <v>0.434722135196481</v>
+        <v>0.4347221351963342</v>
       </c>
       <c r="E124">
-        <v>0.4343968068435264</v>
+        <v>0.4343968068435266</v>
       </c>
       <c r="F124">
-        <v>0.4638640230526202</v>
+        <v>0.4638640232145162</v>
       </c>
       <c r="G124">
-        <v>0.4589387283965972</v>
+        <v>0.4589387283965907</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3255,22 +3255,22 @@
         <v>0.430903942</v>
       </c>
       <c r="B125">
-        <v>0.8439876172029182</v>
+        <v>0.8439876171520723</v>
       </c>
       <c r="C125">
-        <v>0.9137206145558987</v>
+        <v>0.9137206144155456</v>
       </c>
       <c r="D125">
-        <v>0.8753616172221402</v>
+        <v>0.875361617221756</v>
       </c>
       <c r="E125">
-        <v>0.8746670221519124</v>
+        <v>0.8746670221519126</v>
       </c>
       <c r="F125">
-        <v>0.9087208206996762</v>
+        <v>0.9087208210008961</v>
       </c>
       <c r="G125">
-        <v>0.8999921090239356</v>
+        <v>0.8999921090239236</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3278,22 +3278,22 @@
         <v>-0.243546309</v>
       </c>
       <c r="B126">
-        <v>-0.07583556289543836</v>
+        <v>-0.07583556108168893</v>
       </c>
       <c r="C126">
-        <v>0.008616048428981758</v>
+        <v>0.008616048410380824</v>
       </c>
       <c r="D126">
-        <v>-0.0454266780818281</v>
+        <v>-0.04542667808157531</v>
       </c>
       <c r="E126">
-        <v>-0.04183281819723991</v>
+        <v>-0.04183281819723968</v>
       </c>
       <c r="F126">
-        <v>0.008981782956438877</v>
+        <v>0.008981782974863226</v>
       </c>
       <c r="G126">
-        <v>0.006720923291284132</v>
+        <v>0.006720923291283258</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3301,22 +3301,22 @@
         <v>-0.931687809</v>
       </c>
       <c r="B127">
-        <v>-0.9851676318888647</v>
+        <v>-0.9851676287888931</v>
       </c>
       <c r="C127">
-        <v>-0.9075512055043539</v>
+        <v>-0.9075512053119118</v>
       </c>
       <c r="D127">
-        <v>-0.9565929258243512</v>
+        <v>-0.9565929258235214</v>
       </c>
       <c r="E127">
-        <v>-0.9635408098732934</v>
+        <v>-0.9635408098732933</v>
       </c>
       <c r="F127">
-        <v>-0.9032943606168117</v>
+        <v>-0.9032943608816181</v>
       </c>
       <c r="G127">
-        <v>-0.8882266027273097</v>
+        <v>-0.8882266027272993</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3324,22 +3324,22 @@
         <v>0.141116369</v>
       </c>
       <c r="B128">
-        <v>0.0731406230316283</v>
+        <v>0.07314062434255175</v>
       </c>
       <c r="C128">
-        <v>0.1440938787032021</v>
+        <v>0.1440938786723752</v>
       </c>
       <c r="D128">
-        <v>0.06775236283315395</v>
+        <v>0.06775236283344864</v>
       </c>
       <c r="E128">
-        <v>0.07757799321162065</v>
+        <v>0.07757799321162095</v>
       </c>
       <c r="F128">
-        <v>0.1454246986824616</v>
+        <v>0.145424698743702</v>
       </c>
       <c r="G128">
-        <v>0.1410596719559405</v>
+        <v>0.1410596719559379</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3347,22 +3347,22 @@
         <v>0.56391939</v>
       </c>
       <c r="B129">
-        <v>0.5176311987028471</v>
+        <v>0.5176311989286843</v>
       </c>
       <c r="C129">
-        <v>0.5819502406301199</v>
+        <v>0.5819502405172543</v>
       </c>
       <c r="D129">
-        <v>0.4966474744786731</v>
+        <v>0.4966474744787379</v>
       </c>
       <c r="E129">
-        <v>0.4998804091561443</v>
+        <v>0.4998804091561447</v>
       </c>
       <c r="F129">
-        <v>0.57630449718137</v>
+        <v>0.5763044973788268</v>
       </c>
       <c r="G129">
-        <v>0.5707559490502818</v>
+        <v>0.5707559490502738</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -3370,22 +3370,22 @@
         <v>1.941603295</v>
       </c>
       <c r="B130">
-        <v>1.797427551000491</v>
+        <v>1.797427546851027</v>
       </c>
       <c r="C130">
-        <v>1.792946947007821</v>
+        <v>1.792946946769245</v>
       </c>
       <c r="D130">
-        <v>1.720727418399458</v>
+        <v>1.720727418398734</v>
       </c>
       <c r="E130">
         <v>1.720053163289672</v>
       </c>
       <c r="F130">
-        <v>1.786186129395018</v>
+        <v>1.786186129971514</v>
       </c>
       <c r="G130">
-        <v>1.769833694971281</v>
+        <v>1.769833694971257</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -3393,22 +3393,22 @@
         <v>0.686945786</v>
       </c>
       <c r="B131">
-        <v>0.7600987938340278</v>
+        <v>0.7600987933114342</v>
       </c>
       <c r="C131">
-        <v>0.8234382755272744</v>
+        <v>0.8234382753747083</v>
       </c>
       <c r="D131">
-        <v>0.7463440552798255</v>
+        <v>0.7463440552796954</v>
       </c>
       <c r="E131">
-        <v>0.7475006537558868</v>
+        <v>0.747500653755887</v>
       </c>
       <c r="F131">
-        <v>0.816012134630191</v>
+        <v>0.8160121349024346</v>
       </c>
       <c r="G131">
-        <v>0.8083261992012091</v>
+        <v>0.8083261992011982</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -3416,22 +3416,22 @@
         <v>0.489776809</v>
       </c>
       <c r="B132">
-        <v>1.109625557966213</v>
+        <v>1.109625556100302</v>
       </c>
       <c r="C132">
-        <v>1.160032734441135</v>
+        <v>1.160032734242288</v>
       </c>
       <c r="D132">
-        <v>1.077871908694663</v>
+        <v>1.077871908694356</v>
       </c>
       <c r="E132">
         <v>1.078348160551975</v>
       </c>
       <c r="F132">
-        <v>1.151298376027326</v>
+        <v>1.151298376404528</v>
       </c>
       <c r="G132">
-        <v>1.140414037417566</v>
+        <v>1.140414037417551</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3439,22 +3439,22 @@
         <v>-0.927615797</v>
       </c>
       <c r="B133">
-        <v>0.006553849437508596</v>
+        <v>0.006553851352811211</v>
       </c>
       <c r="C133">
-        <v>0.1228675378209579</v>
+        <v>0.1228675377773724</v>
       </c>
       <c r="D133">
-        <v>0.0519602860169724</v>
+        <v>0.05196028601724384</v>
       </c>
       <c r="E133">
-        <v>0.05459802866931435</v>
+        <v>0.0545980286693146</v>
       </c>
       <c r="F133">
-        <v>0.120863102452846</v>
+        <v>0.1208631025061702</v>
       </c>
       <c r="G133">
-        <v>0.1184653142487897</v>
+        <v>0.1184653142487875</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3462,22 +3462,22 @@
         <v>-0.570785532</v>
       </c>
       <c r="B134">
-        <v>-0.0008408148582552347</v>
+        <v>-0.0008408127219168221</v>
       </c>
       <c r="C134">
-        <v>0.1181385917639832</v>
+        <v>0.1181385917195056</v>
       </c>
       <c r="D134">
-        <v>0.05816426765554331</v>
+        <v>0.05816426765575701</v>
       </c>
       <c r="E134">
-        <v>0.06008080227591712</v>
+        <v>0.06008080227591735</v>
       </c>
       <c r="F134">
-        <v>0.1159551333991878</v>
+        <v>0.1159551334510149</v>
       </c>
       <c r="G134">
-        <v>0.1136374006455827</v>
+        <v>0.1136374006455805</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -3485,22 +3485,22 @@
         <v>0.629936161</v>
       </c>
       <c r="B135">
-        <v>0.1603070432227465</v>
+        <v>0.16030704481354</v>
       </c>
       <c r="C135">
-        <v>0.2608445833251528</v>
+        <v>0.2608445832555576</v>
       </c>
       <c r="D135">
-        <v>0.2175882917392751</v>
+        <v>0.2175882917393073</v>
       </c>
       <c r="E135">
-        <v>0.2183711982401299</v>
+        <v>0.2183711982401301</v>
       </c>
       <c r="F135">
-        <v>0.2572734091846444</v>
+        <v>0.2572734092808652</v>
       </c>
       <c r="G135">
-        <v>0.253854368465699</v>
+        <v>0.2538543684656951</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -3508,22 +3508,22 @@
         <v>1.229927464</v>
       </c>
       <c r="B136">
-        <v>1.03700217876511</v>
+        <v>1.037002178700838</v>
       </c>
       <c r="C136">
-        <v>1.116249326970873</v>
+        <v>1.116249326818573</v>
       </c>
       <c r="D136">
-        <v>1.083485896291935</v>
+        <v>1.083485896291404</v>
       </c>
       <c r="E136">
         <v>1.082169313305273</v>
       </c>
       <c r="F136">
-        <v>1.112011329268558</v>
+        <v>1.112011329633981</v>
       </c>
       <c r="G136">
-        <v>1.101484204208677</v>
+        <v>1.101484204208662</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -3531,22 +3531,22 @@
         <v>0.831135585</v>
       </c>
       <c r="B137">
-        <v>0.5537135766096237</v>
+        <v>0.5537135771143457</v>
       </c>
       <c r="C137">
-        <v>0.6282613947006174</v>
+        <v>0.628261394586705</v>
       </c>
       <c r="D137">
-        <v>0.587108696937508</v>
+        <v>0.5871086969373068</v>
       </c>
       <c r="E137">
-        <v>0.5870492003231762</v>
+        <v>0.5870492003231765</v>
       </c>
       <c r="F137">
-        <v>0.6232830320652509</v>
+        <v>0.6232830322767642</v>
       </c>
       <c r="G137">
-        <v>0.6170058868841616</v>
+        <v>0.6170058868841531</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -3554,22 +3554,22 @@
         <v>-0.615633494</v>
       </c>
       <c r="B138">
-        <v>-0.2884491046602247</v>
+        <v>-0.2884491024204741</v>
       </c>
       <c r="C138">
-        <v>-0.2022115984864537</v>
+        <v>-0.2022115984638043</v>
       </c>
       <c r="D138">
-        <v>-0.2546112764092172</v>
+        <v>-0.2546112764088382</v>
       </c>
       <c r="E138">
-        <v>-0.2482192862838705</v>
+        <v>-0.2482192862838703</v>
       </c>
       <c r="F138">
-        <v>-0.1975414179097126</v>
+        <v>-0.197541417956839</v>
       </c>
       <c r="G138">
-        <v>-0.1999935406353604</v>
+        <v>-0.1999935406353587</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -3577,22 +3577,22 @@
         <v>-0.504548817</v>
       </c>
       <c r="B139">
-        <v>-0.5635677124937828</v>
+        <v>-0.5635677100580835</v>
       </c>
       <c r="C139">
-        <v>-0.4833372476191662</v>
+        <v>-0.4833372475310305</v>
       </c>
       <c r="D139">
-        <v>-0.5406772280581116</v>
+        <v>-0.5406772280575195</v>
       </c>
       <c r="E139">
-        <v>-0.5684058333616513</v>
+        <v>-0.5684058333616511</v>
       </c>
       <c r="F139">
-        <v>-0.4980046293783691</v>
+        <v>-0.4980046295116665</v>
       </c>
       <c r="G139">
-        <v>-0.474531579048928</v>
+        <v>-0.4745315790489228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
goliatt seg dez 13 07:40:07 -03 2021
</commit_message>
<xml_diff>
--- a/table_best_models____spi-3__test.xlsx
+++ b/table_best_models____spi-3__test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Observed</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Lasso ($\beta = $1.5)</t>
+  </si>
+  <si>
+    <t>Lasso ($\beta = $10.0)</t>
   </si>
   <si>
     <t>Lasso ($\beta = $2.0)</t>
@@ -392,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:H139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,8 +423,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>0.798426952</v>
       </c>
@@ -429,7 +435,7 @@
         <v>0.8570327671020751</v>
       </c>
       <c r="C2">
-        <v>0.8674250061198436</v>
+        <v>0.7862415843415023</v>
       </c>
       <c r="D2">
         <v>0.8670854193478963</v>
@@ -441,10 +447,13 @@
         <v>0.867046342060002</v>
       </c>
       <c r="G2">
+        <v>0.6780045251171484</v>
+      </c>
+      <c r="H2">
         <v>0.8592882910984092</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>-0.135008744</v>
       </c>
@@ -452,7 +461,7 @@
         <v>0.7326825141436214</v>
       </c>
       <c r="C3">
-        <v>0.7660749047608373</v>
+        <v>0.6910890989654364</v>
       </c>
       <c r="D3">
         <v>0.7170747516091714</v>
@@ -464,10 +473,13 @@
         <v>0.7593774097772397</v>
       </c>
       <c r="G3">
+        <v>0.5923336103323501</v>
+      </c>
+      <c r="H3">
         <v>0.7523822066406555</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>0.483128577</v>
       </c>
@@ -475,7 +487,7 @@
         <v>0.159937075596327</v>
       </c>
       <c r="C4">
-        <v>0.2109950894471056</v>
+        <v>0.09840151080256659</v>
       </c>
       <c r="D4">
         <v>0.1805269018647896</v>
@@ -487,10 +499,13 @@
         <v>0.2069589468302485</v>
       </c>
       <c r="G4">
+        <v>0.1534455544834205</v>
+      </c>
+      <c r="H4">
         <v>0.2038624479992588</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>0.358803155</v>
       </c>
@@ -498,7 +513,7 @@
         <v>-0.4226666300367006</v>
       </c>
       <c r="C5">
-        <v>-0.3115414410878165</v>
+        <v>-0.4612805883162602</v>
       </c>
       <c r="D5">
         <v>-0.3805194157057444</v>
@@ -510,10 +525,13 @@
         <v>-0.3145528386299085</v>
       </c>
       <c r="G5">
+        <v>-0.2561896164741698</v>
+      </c>
+      <c r="H5">
         <v>-0.3147940136636487</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>0.9297649529999999</v>
       </c>
@@ -521,7 +539,7 @@
         <v>0.1366489192602485</v>
       </c>
       <c r="C6">
-        <v>0.2161612459445032</v>
+        <v>0.1046285417443273</v>
       </c>
       <c r="D6">
         <v>0.1465630873630199</v>
@@ -533,10 +551,13 @@
         <v>0.2110634080120473</v>
       </c>
       <c r="G6">
+        <v>0.1574117787639404</v>
+      </c>
+      <c r="H6">
         <v>0.2081327957465628</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>-0.343866365</v>
       </c>
@@ -544,7 +565,7 @@
         <v>-0.6055685168215885</v>
       </c>
       <c r="C7">
-        <v>-0.5478437317397367</v>
+        <v>-0.6021960799080008</v>
       </c>
       <c r="D7">
         <v>-0.5873153748257482</v>
@@ -556,10 +577,13 @@
         <v>-0.5395843899572571</v>
       </c>
       <c r="G7">
+        <v>-0.4416496932881392</v>
+      </c>
+      <c r="H7">
         <v>-0.542376023180689</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>-0.394869887</v>
       </c>
@@ -567,7 +591,7 @@
         <v>-0.354401351100021</v>
       </c>
       <c r="C8">
-        <v>-0.25623798896717</v>
+        <v>-0.3064320962304403</v>
       </c>
       <c r="D8">
         <v>-0.2911052084763237</v>
@@ -579,10 +603,13 @@
         <v>-0.2571016599835869</v>
       </c>
       <c r="G8">
+        <v>-0.2142648226272789</v>
+      </c>
+      <c r="H8">
         <v>-0.256599629285902</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>0.124976886</v>
       </c>
@@ -590,7 +617,7 @@
         <v>0.4065369392719085</v>
       </c>
       <c r="C9">
-        <v>0.4550571593413335</v>
+        <v>0.4279044728572459</v>
       </c>
       <c r="D9">
         <v>0.443639197244627</v>
@@ -602,10 +629,13 @@
         <v>0.4512238387534177</v>
       </c>
       <c r="G9">
+        <v>0.3459947103809031</v>
+      </c>
+      <c r="H9">
         <v>0.4462374925194611</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>0.714385868</v>
       </c>
@@ -613,7 +643,7 @@
         <v>0.8459672685817484</v>
       </c>
       <c r="C10">
-        <v>0.8863712726228958</v>
+        <v>0.8581036468350874</v>
       </c>
       <c r="D10">
         <v>0.8804605020652532</v>
@@ -625,10 +655,13 @@
         <v>0.8852831170688441</v>
       </c>
       <c r="G10">
+        <v>0.6893326538954757</v>
+      </c>
+      <c r="H10">
         <v>0.876112736756281</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>0.495936019</v>
       </c>
@@ -636,7 +669,7 @@
         <v>0.5114182901811332</v>
       </c>
       <c r="C11">
-        <v>0.5326541335343883</v>
+        <v>0.5173154905226341</v>
       </c>
       <c r="D11">
         <v>0.5056704980129281</v>
@@ -648,10 +681,13 @@
         <v>0.5276060656096382</v>
       </c>
       <c r="G11">
+        <v>0.4087809572881352</v>
+      </c>
+      <c r="H11">
         <v>0.5225599813036644</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>-1.049232267</v>
       </c>
@@ -659,7 +695,7 @@
         <v>-0.8549446305690328</v>
       </c>
       <c r="C12">
-        <v>-0.8548170791291492</v>
+        <v>-0.9304620839677633</v>
       </c>
       <c r="D12">
         <v>-0.8861227154463175</v>
@@ -671,10 +707,13 @@
         <v>-0.8584596352192811</v>
       </c>
       <c r="G12">
+        <v>-0.6815337851397134</v>
+      </c>
+      <c r="H12">
         <v>-0.8441335123158428</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>-0.962528123</v>
       </c>
@@ -682,7 +721,7 @@
         <v>-0.5508499193587389</v>
       </c>
       <c r="C13">
-        <v>-0.5588304447962913</v>
+        <v>-0.6745069172646256</v>
       </c>
       <c r="D13">
         <v>-0.608779505325819</v>
@@ -694,10 +733,13 @@
         <v>-0.5558074253001822</v>
       </c>
       <c r="G13">
+        <v>-0.4493081436357848</v>
+      </c>
+      <c r="H13">
         <v>-0.5498462501739224</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>-0.823266309</v>
       </c>
@@ -705,7 +747,7 @@
         <v>-0.5387245457306077</v>
       </c>
       <c r="C14">
-        <v>-0.5550114419508775</v>
+        <v>-0.5440954829532499</v>
       </c>
       <c r="D14">
         <v>-0.5556809834796582</v>
@@ -717,10 +759,13 @@
         <v>-0.56500996475396</v>
       </c>
       <c r="G14">
+        <v>-0.4503975538734379</v>
+      </c>
+      <c r="H14">
         <v>-0.5490960969727648</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>-0.566899673</v>
       </c>
@@ -728,7 +773,7 @@
         <v>-0.553569955843472</v>
       </c>
       <c r="C15">
-        <v>-0.4900207760677317</v>
+        <v>-0.4983172244498884</v>
       </c>
       <c r="D15">
         <v>-0.521636565520975</v>
@@ -740,10 +785,13 @@
         <v>-0.5050242796887064</v>
       </c>
       <c r="G15">
+        <v>-0.3970346032304233</v>
+      </c>
+      <c r="H15">
         <v>-0.4863775757637639</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>1.061843082</v>
       </c>
@@ -751,7 +799,7 @@
         <v>0.8567354323737162</v>
       </c>
       <c r="C16">
-        <v>0.9236299545167342</v>
+        <v>0.9360238976626226</v>
       </c>
       <c r="D16">
         <v>0.9431110412191371</v>
@@ -763,10 +811,13 @@
         <v>0.9268183694219724</v>
       </c>
       <c r="G16">
+        <v>0.7222220437371715</v>
+      </c>
+      <c r="H16">
         <v>0.9165914429952459</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>1.223874814</v>
       </c>
@@ -774,7 +825,7 @@
         <v>1.10414363773598</v>
       </c>
       <c r="C17">
-        <v>1.160127196405216</v>
+        <v>1.050747059140312</v>
       </c>
       <c r="D17">
         <v>1.191775102043232</v>
@@ -786,10 +837,13 @@
         <v>1.166977315935523</v>
       </c>
       <c r="G17">
+        <v>0.9118077933205726</v>
+      </c>
+      <c r="H17">
         <v>1.154804837335849</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>1.243571118</v>
       </c>
@@ -797,7 +851,7 @@
         <v>1.047311311849136</v>
       </c>
       <c r="C18">
-        <v>1.094528800430761</v>
+        <v>0.9873249537280578</v>
       </c>
       <c r="D18">
         <v>1.151887156650582</v>
@@ -809,10 +863,13 @@
         <v>1.10552016901935</v>
       </c>
       <c r="G18">
+        <v>0.8637708396115118</v>
+      </c>
+      <c r="H18">
         <v>1.09360734400521</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>-1.371414383</v>
       </c>
@@ -820,7 +877,7 @@
         <v>-1.098086678711034</v>
       </c>
       <c r="C19">
-        <v>-1.153627873825032</v>
+        <v>-1.20776409786106</v>
       </c>
       <c r="D19">
         <v>-1.154633955869579</v>
@@ -832,10 +889,13 @@
         <v>-1.155258192675071</v>
       </c>
       <c r="G19">
+        <v>-0.917963995350717</v>
+      </c>
+      <c r="H19">
         <v>-1.143856610615331</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>-1.6161627</v>
       </c>
@@ -843,7 +903,7 @@
         <v>-1.313066484048699</v>
       </c>
       <c r="C20">
-        <v>-1.283338494593717</v>
+        <v>-1.313759178678514</v>
       </c>
       <c r="D20">
         <v>-1.294166590442324</v>
@@ -855,10 +915,13 @@
         <v>-1.284311627088639</v>
       </c>
       <c r="G20">
+        <v>-1.018239965602924</v>
+      </c>
+      <c r="H20">
         <v>-1.270845046119552</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>-1.663613601</v>
       </c>
@@ -866,7 +929,7 @@
         <v>-1.328883067250665</v>
       </c>
       <c r="C21">
-        <v>-1.246902318176336</v>
+        <v>-1.326083100537944</v>
       </c>
       <c r="D21">
         <v>-1.290393136071035</v>
@@ -878,10 +941,13 @@
         <v>-1.239262441344044</v>
       </c>
       <c r="G21">
+        <v>-0.9846192060692045</v>
+      </c>
+      <c r="H21">
         <v>-1.225460472533575</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>-0.39083508</v>
       </c>
@@ -889,7 +955,7 @@
         <v>-0.4714463925043804</v>
       </c>
       <c r="C22">
-        <v>-0.3902814283717299</v>
+        <v>-0.436636969112735</v>
       </c>
       <c r="D22">
         <v>-0.4298942636056386</v>
@@ -901,10 +967,13 @@
         <v>-0.3891915144401171</v>
       </c>
       <c r="G22">
+        <v>-0.3185995584480339</v>
+      </c>
+      <c r="H22">
         <v>-0.3887655102598211</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>-1.294350414</v>
       </c>
@@ -912,7 +981,7 @@
         <v>-1.351254409315158</v>
       </c>
       <c r="C23">
-        <v>-1.317022201063619</v>
+        <v>-1.368492544380365</v>
       </c>
       <c r="D23">
         <v>-1.355119067495509</v>
@@ -924,10 +993,13 @@
         <v>-1.209489840054009</v>
       </c>
       <c r="G23">
+        <v>-1.038634954746098</v>
+      </c>
+      <c r="H23">
         <v>-1.292098446580037</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>-1.735350123</v>
       </c>
@@ -935,7 +1007,7 @@
         <v>-1.73005320125318</v>
       </c>
       <c r="C24">
-        <v>-1.650744240412817</v>
+        <v>-1.69171314318727</v>
       </c>
       <c r="D24">
         <v>-1.681349034671773</v>
@@ -947,10 +1019,13 @@
         <v>-1.624475121125265</v>
       </c>
       <c r="G24">
+        <v>-1.299063032759233</v>
+      </c>
+      <c r="H24">
         <v>-1.621006673851315</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>-1.464171309</v>
       </c>
@@ -958,7 +1033,7 @@
         <v>-1.31212270298792</v>
       </c>
       <c r="C25">
-        <v>-1.146334238788492</v>
+        <v>-1.208803780880302</v>
       </c>
       <c r="D25">
         <v>-1.195889426588707</v>
@@ -970,10 +1045,13 @@
         <v>-1.003446150075503</v>
       </c>
       <c r="G25">
+        <v>-0.9075835926069729</v>
+      </c>
+      <c r="H25">
         <v>-1.131205458463111</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>-1.138267628</v>
       </c>
@@ -981,7 +1059,7 @@
         <v>-1.287163792983685</v>
       </c>
       <c r="C26">
-        <v>-1.127386481620193</v>
+        <v>-1.191008208490535</v>
       </c>
       <c r="D26">
         <v>-1.178561800766996</v>
@@ -993,10 +1071,13 @@
         <v>-1.130831577260678</v>
       </c>
       <c r="G26">
+        <v>-0.8924484111562536</v>
+      </c>
+      <c r="H26">
         <v>-1.111688043998501</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>-0.231935471</v>
       </c>
@@ -1004,7 +1085,7 @@
         <v>-0.2593559476433276</v>
       </c>
       <c r="C27">
-        <v>-0.1947111996547763</v>
+        <v>-0.2119876535356679</v>
       </c>
       <c r="D27">
         <v>-0.2297985477678169</v>
@@ -1016,10 +1097,13 @@
         <v>-0.1972479020788469</v>
       </c>
       <c r="G27">
+        <v>-0.1649476225312969</v>
+      </c>
+      <c r="H27">
         <v>-0.197792683297428</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>-1.071257154</v>
       </c>
@@ -1027,7 +1111,7 @@
         <v>-1.21423351701524</v>
       </c>
       <c r="C28">
-        <v>-1.238894224575838</v>
+        <v>-1.277944206788346</v>
       </c>
       <c r="D28">
         <v>-1.24692596081704</v>
@@ -1039,10 +1123,13 @@
         <v>-1.238365552526167</v>
       </c>
       <c r="G28">
+        <v>-0.983548360114874</v>
+      </c>
+      <c r="H28">
         <v>-1.224842760852701</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>-0.788753691</v>
       </c>
@@ -1050,7 +1137,7 @@
         <v>-0.7057312816562966</v>
       </c>
       <c r="C29">
-        <v>-0.6705173137256708</v>
+        <v>-0.7440757218171062</v>
       </c>
       <c r="D29">
         <v>-0.7178687858302228</v>
@@ -1062,10 +1149,13 @@
         <v>-0.6692234087625388</v>
       </c>
       <c r="G29">
+        <v>-0.5364753641595498</v>
+      </c>
+      <c r="H29">
         <v>-0.661086718666251</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>0.168216722</v>
       </c>
@@ -1073,7 +1163,7 @@
         <v>0.2964061175682076</v>
       </c>
       <c r="C30">
-        <v>0.3359678813561835</v>
+        <v>0.2856730172998495</v>
       </c>
       <c r="D30">
         <v>0.2847304034400726</v>
@@ -1085,10 +1175,13 @@
         <v>0.3331286982271702</v>
       </c>
       <c r="G30">
+        <v>0.2506008933139455</v>
+      </c>
+      <c r="H30">
         <v>0.3283703672518958</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>0.589617249</v>
       </c>
@@ -1096,7 +1189,7 @@
         <v>1.068030720368563</v>
       </c>
       <c r="C31">
-        <v>1.106263044351173</v>
+        <v>1.051092041793016</v>
       </c>
       <c r="D31">
         <v>1.098698030924074</v>
@@ -1108,10 +1201,13 @@
         <v>1.103776647539465</v>
       </c>
       <c r="G31">
+        <v>0.8604167777788367</v>
+      </c>
+      <c r="H31">
         <v>1.09386685081366</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>0.34764818</v>
       </c>
@@ -1119,7 +1215,7 @@
         <v>0.8119551479412531</v>
       </c>
       <c r="C32">
-        <v>0.8429678232674723</v>
+        <v>0.8086492858652553</v>
       </c>
       <c r="D32">
         <v>0.8287522308706857</v>
@@ -1131,10 +1227,13 @@
         <v>0.8387231490240649</v>
       </c>
       <c r="G32">
+        <v>0.6516345098892038</v>
+      </c>
+      <c r="H32">
         <v>0.8313367682176924</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>-1.151348471</v>
       </c>
@@ -1142,7 +1241,7 @@
         <v>-0.3395585291620783</v>
       </c>
       <c r="C33">
-        <v>-0.3195777983912563</v>
+        <v>-0.3255488936289495</v>
       </c>
       <c r="D33">
         <v>-0.3387822063407494</v>
@@ -1154,10 +1253,13 @@
         <v>-0.3240468484612157</v>
       </c>
       <c r="G33">
+        <v>-0.2639071942713627</v>
+      </c>
+      <c r="H33">
         <v>-0.3203215459971525</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>-0.696093006</v>
       </c>
@@ -1165,7 +1267,7 @@
         <v>-0.7489061106402813</v>
       </c>
       <c r="C34">
-        <v>-0.7126815278583926</v>
+        <v>-0.7422146176808122</v>
       </c>
       <c r="D34">
         <v>-0.7327503452585801</v>
@@ -1177,10 +1279,13 @@
         <v>-0.7285928226752461</v>
       </c>
       <c r="G34">
+        <v>-0.5717042704151685</v>
+      </c>
+      <c r="H34">
         <v>-0.7074657276201931</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>-0.726012958</v>
       </c>
@@ -1188,7 +1293,7 @@
         <v>-0.5187230041998776</v>
       </c>
       <c r="C35">
-        <v>-0.4822834272884639</v>
+        <v>-0.5012739962334104</v>
       </c>
       <c r="D35">
         <v>-0.4909911580284282</v>
@@ -1200,10 +1305,13 @@
         <v>-0.4826126074950333</v>
       </c>
       <c r="G35">
+        <v>-0.3917178482547591</v>
+      </c>
+      <c r="H35">
         <v>-0.4817098444962419</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>-0.087224411</v>
       </c>
@@ -1211,7 +1319,7 @@
         <v>-0.2709417015515872</v>
       </c>
       <c r="C36">
-        <v>-0.2349725323167318</v>
+        <v>-0.255292057701359</v>
       </c>
       <c r="D36">
         <v>-0.228886230554961</v>
@@ -1223,10 +1331,13 @@
         <v>-0.237963376291208</v>
       </c>
       <c r="G36">
+        <v>-0.1972848749136212</v>
+      </c>
+      <c r="H36">
         <v>-0.2379035261165182</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>-1.025152274</v>
       </c>
@@ -1234,7 +1345,7 @@
         <v>-0.7792852571960617</v>
       </c>
       <c r="C37">
-        <v>-0.7977091660328214</v>
+        <v>-0.8251524696986997</v>
       </c>
       <c r="D37">
         <v>-0.8064753824936667</v>
@@ -1246,10 +1357,13 @@
         <v>-0.8073486099274139</v>
       </c>
       <c r="G37">
+        <v>-0.6392405496074858</v>
+      </c>
+      <c r="H37">
         <v>-0.7902624739898323</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>-1.065636548</v>
       </c>
@@ -1257,7 +1371,7 @@
         <v>-0.9175001852746184</v>
       </c>
       <c r="C38">
-        <v>-0.9444270817803803</v>
+        <v>-0.9876754773760315</v>
       </c>
       <c r="D38">
         <v>-0.9622365604693761</v>
@@ -1269,10 +1383,13 @@
         <v>-0.9438475219908058</v>
       </c>
       <c r="G38">
+        <v>-0.7524959855787268</v>
+      </c>
+      <c r="H38">
         <v>-0.9320792423529037</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>-1.658517568</v>
       </c>
@@ -1280,7 +1397,7 @@
         <v>-0.9921205694088507</v>
       </c>
       <c r="C39">
-        <v>-0.9599469514526012</v>
+        <v>-1.023451382482716</v>
       </c>
       <c r="D39">
         <v>-1.004865794004151</v>
@@ -1292,10 +1409,13 @@
         <v>-0.9530528558203429</v>
       </c>
       <c r="G39">
+        <v>-0.7611674580807017</v>
+      </c>
+      <c r="H39">
         <v>-0.9430513160342175</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>0.670350201</v>
       </c>
@@ -1303,7 +1423,7 @@
         <v>0.371577793643929</v>
       </c>
       <c r="C40">
-        <v>0.372947970033949</v>
+        <v>0.418587698298642</v>
       </c>
       <c r="D40">
         <v>0.3575056405256379</v>
@@ -1315,10 +1435,13 @@
         <v>0.3693166368247627</v>
       </c>
       <c r="G40">
+        <v>0.2851204273449287</v>
+      </c>
+      <c r="H40">
         <v>0.3649757325805749</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>0.58174072</v>
       </c>
@@ -1326,7 +1449,7 @@
         <v>0.384771805074932</v>
       </c>
       <c r="C41">
-        <v>0.381072866841321</v>
+        <v>0.4292728801360066</v>
       </c>
       <c r="D41">
         <v>0.3590180041027327</v>
@@ -1338,10 +1461,13 @@
         <v>0.3750690623814169</v>
       </c>
       <c r="G41">
+        <v>0.2896184844778754</v>
+      </c>
+      <c r="H41">
         <v>0.3724216873541051</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>1.034492187</v>
       </c>
@@ -1349,7 +1475,7 @@
         <v>0.6990552402781258</v>
       </c>
       <c r="C42">
-        <v>0.712194475848672</v>
+        <v>0.7193234509314015</v>
       </c>
       <c r="D42">
         <v>0.7046705388873978</v>
@@ -1361,10 +1487,13 @@
         <v>0.7097799562094962</v>
       </c>
       <c r="G42">
+        <v>0.551589658395269</v>
+      </c>
+      <c r="H42">
         <v>0.7026052882596869</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>-0.330510864</v>
       </c>
@@ -1372,7 +1501,7 @@
         <v>-0.3090539206985012</v>
       </c>
       <c r="C43">
-        <v>-0.2664560677873326</v>
+        <v>-0.3156900230488798</v>
       </c>
       <c r="D43">
         <v>-0.3206383739029788</v>
@@ -1384,10 +1513,13 @@
         <v>-0.2682391849531642</v>
       </c>
       <c r="G43">
+        <v>-0.2177825511188773</v>
+      </c>
+      <c r="H43">
         <v>-0.2640666716670347</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>0.468647097</v>
       </c>
@@ -1395,7 +1527,7 @@
         <v>0.421273519793997</v>
       </c>
       <c r="C44">
-        <v>0.5082044799143509</v>
+        <v>0.4183824170844823</v>
       </c>
       <c r="D44">
         <v>0.4986448681723796</v>
@@ -1407,10 +1539,13 @@
         <v>0.5049118878207794</v>
       </c>
       <c r="G44">
+        <v>0.3881233265235815</v>
+      </c>
+      <c r="H44">
         <v>0.4990974832365626</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>1.030934397</v>
       </c>
@@ -1418,7 +1553,7 @@
         <v>1.472937177743613</v>
       </c>
       <c r="C45">
-        <v>1.5571979530129</v>
+        <v>1.48607683217392</v>
       </c>
       <c r="D45">
         <v>1.588675048882149</v>
@@ -1430,10 +1565,13 @@
         <v>1.566868159006285</v>
       </c>
       <c r="G45">
+        <v>1.226147984803601</v>
+      </c>
+      <c r="H45">
         <v>1.551243771826003</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>1.479112841</v>
       </c>
@@ -1441,7 +1579,7 @@
         <v>1.962117044607471</v>
       </c>
       <c r="C46">
-        <v>2.02281777939433</v>
+        <v>2.003178588377591</v>
       </c>
       <c r="D46">
         <v>2.08976685583256</v>
@@ -1453,10 +1591,13 @@
         <v>2.048490944459196</v>
       </c>
       <c r="G46">
+        <v>1.606757066648953</v>
+      </c>
+      <c r="H46">
         <v>2.027972967651845</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>1.817472853</v>
       </c>
@@ -1464,7 +1605,7 @@
         <v>2.269973697488466</v>
       </c>
       <c r="C47">
-        <v>2.277103438043807</v>
+        <v>2.312607402982944</v>
       </c>
       <c r="D47">
         <v>2.339561150242502</v>
@@ -1476,10 +1617,13 @@
         <v>2.304864303290234</v>
       </c>
       <c r="G47">
+        <v>1.80880973497463</v>
+      </c>
+      <c r="H47">
         <v>2.282422043352537</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>0.369717394</v>
       </c>
@@ -1487,7 +1631,7 @@
         <v>0.7936619029909401</v>
       </c>
       <c r="C48">
-        <v>0.8246021676002975</v>
+        <v>0.7423288215927401</v>
       </c>
       <c r="D48">
         <v>0.8430871754160236</v>
@@ -1499,10 +1643,13 @@
         <v>0.8242501691819413</v>
       </c>
       <c r="G48">
+        <v>0.6410770829557343</v>
+      </c>
+      <c r="H48">
         <v>0.816309162843404</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>-0.162350195</v>
       </c>
@@ -1510,7 +1657,7 @@
         <v>-0.07979008564074222</v>
       </c>
       <c r="C49">
-        <v>-0.1196113210778009</v>
+        <v>-0.1250085043873634</v>
       </c>
       <c r="D49">
         <v>-0.09012291515904616</v>
@@ -1522,10 +1669,13 @@
         <v>-0.1218664408219997</v>
       </c>
       <c r="G49">
+        <v>-0.1053019177823357</v>
+      </c>
+      <c r="H49">
         <v>-0.1234465852809974</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50">
         <v>-0.729825744</v>
       </c>
@@ -1533,7 +1683,7 @@
         <v>-0.8392456283653114</v>
       </c>
       <c r="C50">
-        <v>-0.9340820165572218</v>
+        <v>-0.9516881166947752</v>
       </c>
       <c r="D50">
         <v>-0.904063681863421</v>
@@ -1545,10 +1695,13 @@
         <v>-0.9357186711316287</v>
       </c>
       <c r="G50">
+        <v>-0.747151104354328</v>
+      </c>
+      <c r="H50">
         <v>-0.9315286757188824</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>-0.317430882</v>
       </c>
@@ -1556,7 +1709,7 @@
         <v>-0.7801388757159254</v>
       </c>
       <c r="C51">
-        <v>-0.8409457176747623</v>
+        <v>-0.8739363687864342</v>
       </c>
       <c r="D51">
         <v>-0.817406560151447</v>
@@ -1568,10 +1721,13 @@
         <v>-0.842953795373012</v>
       </c>
       <c r="G51">
+        <v>-0.6728520747273897</v>
+      </c>
+      <c r="H51">
         <v>-0.8389860725881373</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="A52">
         <v>-0.490640104</v>
       </c>
@@ -1579,7 +1735,7 @@
         <v>-0.689039284000471</v>
       </c>
       <c r="C52">
-        <v>-0.7046779807546086</v>
+        <v>-0.7320397800162977</v>
       </c>
       <c r="D52">
         <v>-0.6846239450980729</v>
@@ -1591,10 +1747,13 @@
         <v>-0.7067700195871465</v>
       </c>
       <c r="G52">
+        <v>-0.5633668499563615</v>
+      </c>
+      <c r="H52">
         <v>-0.7036950152242181</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="A53">
         <v>-1.100609032</v>
       </c>
@@ -1602,7 +1761,7 @@
         <v>-0.9916440899478505</v>
       </c>
       <c r="C53">
-        <v>-0.9855289939775276</v>
+        <v>-1.044521823491443</v>
       </c>
       <c r="D53">
         <v>-1.001032703824808</v>
@@ -1614,10 +1773,13 @@
         <v>-0.9867710923713263</v>
       </c>
       <c r="G53">
+        <v>-0.7852382837358383</v>
+      </c>
+      <c r="H53">
         <v>-0.9777825800431964</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="A54">
         <v>-0.351083172</v>
       </c>
@@ -1625,7 +1787,7 @@
         <v>-0.2309549445506254</v>
       </c>
       <c r="C54">
-        <v>-0.2479094776412257</v>
+        <v>-0.2428784379095458</v>
       </c>
       <c r="D54">
         <v>-0.2375957106564875</v>
@@ -1637,10 +1799,13 @@
         <v>-0.2510954254564975</v>
       </c>
       <c r="G54">
+        <v>-0.2063147147239889</v>
+      </c>
+      <c r="H54">
         <v>-0.2507989467217517</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="A55">
         <v>0.476992209</v>
       </c>
@@ -1648,7 +1813,7 @@
         <v>0.8381025466593807</v>
       </c>
       <c r="C55">
-        <v>0.855895343430586</v>
+        <v>0.8047770121829595</v>
       </c>
       <c r="D55">
         <v>0.8942094393436996</v>
@@ -1660,10 +1825,13 @@
         <v>0.8575928422175573</v>
       </c>
       <c r="G55">
+        <v>0.6674298825568642</v>
+      </c>
+      <c r="H55">
         <v>0.8493834402192112</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>1.269210822</v>
       </c>
@@ -1671,7 +1839,7 @@
         <v>1.516892656630009</v>
       </c>
       <c r="C56">
-        <v>1.581149966837677</v>
+        <v>1.491200839044807</v>
       </c>
       <c r="D56">
         <v>1.618554980232208</v>
@@ -1683,10 +1851,13 @@
         <v>1.590061245600913</v>
       </c>
       <c r="G56">
+        <v>1.244126493293999</v>
+      </c>
+      <c r="H56">
         <v>1.574922717260364</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:8">
       <c r="A57">
         <v>1.68335771</v>
       </c>
@@ -1694,7 +1865,7 @@
         <v>1.752196266474676</v>
       </c>
       <c r="C57">
-        <v>1.779347353792924</v>
+        <v>1.736448829980986</v>
       </c>
       <c r="D57">
         <v>1.836066513996483</v>
@@ -1706,10 +1877,13 @@
         <v>1.795965199337737</v>
       </c>
       <c r="G57">
+        <v>1.407320935119185</v>
+      </c>
+      <c r="H57">
         <v>1.778749688035567</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:8">
       <c r="A58">
         <v>1.248614285</v>
       </c>
@@ -1717,7 +1891,7 @@
         <v>1.289715001335042</v>
       </c>
       <c r="C58">
-        <v>1.31731475970882</v>
+        <v>1.253416307977672</v>
       </c>
       <c r="D58">
         <v>1.334354467821395</v>
@@ -1729,10 +1903,13 @@
         <v>1.321763445606126</v>
       </c>
       <c r="G58">
+        <v>1.033543781136455</v>
+      </c>
+      <c r="H58">
         <v>1.309013353596577</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:8">
       <c r="A59">
         <v>0.747520063</v>
       </c>
@@ -1740,7 +1917,7 @@
         <v>0.6742730445647642</v>
       </c>
       <c r="C59">
-        <v>0.7153969204902284</v>
+        <v>0.6426227743981898</v>
       </c>
       <c r="D59">
         <v>0.7412501308629188</v>
@@ -1752,10 +1929,13 @@
         <v>0.7166668488232818</v>
       </c>
       <c r="G59">
+        <v>0.5564325139043511</v>
+      </c>
+      <c r="H59">
         <v>0.7087772430700017</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:8">
       <c r="A60">
         <v>-0.631971431</v>
       </c>
@@ -1763,7 +1943,7 @@
         <v>-0.4451684906212131</v>
       </c>
       <c r="C60">
-        <v>-0.4820944398350928</v>
+        <v>-0.5506628215857841</v>
       </c>
       <c r="D60">
         <v>-0.4740257692458545</v>
@@ -1775,10 +1955,13 @@
         <v>-0.4835780988744101</v>
       </c>
       <c r="G60">
+        <v>-0.3926148539277185</v>
+      </c>
+      <c r="H60">
         <v>-0.4822972224904558</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:8">
       <c r="A61">
         <v>-0.10813702</v>
       </c>
@@ -1786,7 +1969,7 @@
         <v>0.1542563164794359</v>
       </c>
       <c r="C61">
-        <v>0.1759877440878156</v>
+        <v>0.1211928156847434</v>
       </c>
       <c r="D61">
         <v>0.1741275484797648</v>
@@ -1798,10 +1981,13 @@
         <v>0.17223051120973</v>
       </c>
       <c r="G61">
+        <v>0.1261830464828454</v>
+      </c>
+      <c r="H61">
         <v>0.1696521777234053</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:8">
       <c r="A62">
         <v>0.399434913</v>
       </c>
@@ -1809,7 +1995,7 @@
         <v>0.6451773733723996</v>
       </c>
       <c r="C62">
-        <v>0.6791860626267677</v>
+        <v>0.5876123362951626</v>
       </c>
       <c r="D62">
         <v>0.6692729622792705</v>
@@ -1821,10 +2007,13 @@
         <v>0.6749425685300687</v>
       </c>
       <c r="G62">
+        <v>0.5234860055265023</v>
+      </c>
+      <c r="H62">
         <v>0.6690401321895635</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>0.598079881</v>
       </c>
@@ -1832,7 +2021,7 @@
         <v>0.8046347817200119</v>
       </c>
       <c r="C63">
-        <v>0.8870830148466634</v>
+        <v>0.7353274374938938</v>
       </c>
       <c r="D63">
         <v>0.8521195437018885</v>
@@ -1844,10 +2033,13 @@
         <v>0.8825433160343366</v>
       </c>
       <c r="G63">
+        <v>0.6856552917809342</v>
+      </c>
+      <c r="H63">
         <v>0.8737775699229072</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:8">
       <c r="A64">
         <v>-0.364643642</v>
       </c>
@@ -1855,7 +2047,7 @@
         <v>-0.1509111654828283</v>
       </c>
       <c r="C64">
-        <v>-0.1247233924092499</v>
+        <v>-0.2218333127390271</v>
       </c>
       <c r="D64">
         <v>-0.1484772770734795</v>
@@ -1867,10 +2059,13 @@
         <v>-0.1255883765899089</v>
       </c>
       <c r="G64">
+        <v>-0.1115586299488449</v>
+      </c>
+      <c r="H64">
         <v>-0.125747641701395</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:8">
       <c r="A65">
         <v>2.015990384</v>
       </c>
@@ -1878,7 +2073,7 @@
         <v>1.676061457123847</v>
       </c>
       <c r="C65">
-        <v>1.825354429608222</v>
+        <v>1.844113824627409</v>
       </c>
       <c r="D65">
         <v>1.856629404640485</v>
@@ -1890,10 +2085,13 @@
         <v>1.838084373051688</v>
       </c>
       <c r="G65">
+        <v>1.439463691172252</v>
+      </c>
+      <c r="H65">
         <v>1.819752804076536</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:8">
       <c r="A66">
         <v>2.364869298</v>
       </c>
@@ -1901,7 +2099,7 @@
         <v>1.743513923175322</v>
       </c>
       <c r="C66">
-        <v>1.900760409604738</v>
+        <v>1.937550652973413</v>
       </c>
       <c r="D66">
         <v>1.939276325966659</v>
@@ -1913,10 +2111,13 @@
         <v>1.916100870356827</v>
       </c>
       <c r="G66">
+        <v>1.501039630513977</v>
+      </c>
+      <c r="H66">
         <v>1.896963291773259</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:8">
       <c r="A67">
         <v>2.827580557</v>
       </c>
@@ -1924,7 +2125,7 @@
         <v>1.94848923584483</v>
       </c>
       <c r="C67">
-        <v>2.106841398333119</v>
+        <v>2.062727110715392</v>
       </c>
       <c r="D67">
         <v>2.118018559530195</v>
@@ -1936,10 +2137,13 @@
         <v>2.119046567756093</v>
       </c>
       <c r="G67">
+        <v>1.660784372771637</v>
+      </c>
+      <c r="H67">
         <v>2.09820907680987</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:8">
       <c r="A68">
         <v>0.626809444</v>
       </c>
@@ -1947,7 +2151,7 @@
         <v>0.4416979992316076</v>
       </c>
       <c r="C68">
-        <v>0.4655231901455906</v>
+        <v>0.3735986772796144</v>
       </c>
       <c r="D68">
         <v>0.4517003655389202</v>
@@ -1959,10 +2163,13 @@
         <v>0.4604046196543595</v>
       </c>
       <c r="G68">
+        <v>0.3526006421831478</v>
+      </c>
+      <c r="H68">
         <v>0.4565660743498295</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:8">
       <c r="A69">
         <v>0.49739888</v>
       </c>
@@ -1970,7 +2177,7 @@
         <v>0.3572037886499202</v>
       </c>
       <c r="C69">
-        <v>0.3872810530568308</v>
+        <v>0.2954511434737029</v>
       </c>
       <c r="D69">
         <v>0.3545279425423556</v>
@@ -1982,10 +2189,13 @@
         <v>0.3817891553766893</v>
       </c>
       <c r="G69">
+        <v>0.291032024565865</v>
+      </c>
+      <c r="H69">
         <v>0.3788691845406723</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:8">
       <c r="A70">
         <v>0.325808278</v>
       </c>
@@ -1993,7 +2203,7 @@
         <v>-0.01045030139700145</v>
       </c>
       <c r="C70">
-        <v>0.01489432947952843</v>
+        <v>-0.01494712518755394</v>
       </c>
       <c r="D70">
         <v>-0.030157013039634</v>
@@ -2005,10 +2215,13 @@
         <v>0.01153541867202658</v>
       </c>
       <c r="G70">
+        <v>-0.0008022959364563167</v>
+      </c>
+      <c r="H70">
         <v>0.01118800888669317</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:8">
       <c r="A71">
         <v>0.365489314</v>
       </c>
@@ -2016,7 +2229,7 @@
         <v>0.03554397932472505</v>
       </c>
       <c r="C71">
-        <v>0.09649987835522517</v>
+        <v>0.08435411318088823</v>
       </c>
       <c r="D71">
         <v>0.04953965919820952</v>
@@ -2028,10 +2241,13 @@
         <v>0.09276095691311487</v>
       </c>
       <c r="G71">
+        <v>0.06378000056264149</v>
+      </c>
+      <c r="H71">
         <v>0.09056100580139229</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:8">
       <c r="A72">
         <v>1.026844468</v>
       </c>
@@ -2039,7 +2255,7 @@
         <v>0.6273818103432567</v>
       </c>
       <c r="C72">
-        <v>0.7054266904476194</v>
+        <v>0.6173071729790147</v>
       </c>
       <c r="D72">
         <v>0.6939088747625554</v>
@@ -2051,10 +2267,13 @@
         <v>0.7032786908978439</v>
       </c>
       <c r="G72">
+        <v>0.5455861143203751</v>
+      </c>
+      <c r="H72">
         <v>0.6954052015705211</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:8">
       <c r="A73">
         <v>0.699083059</v>
       </c>
@@ -2062,7 +2281,7 @@
         <v>0.5490537669410885</v>
       </c>
       <c r="C73">
-        <v>0.6068633873298898</v>
+        <v>0.5289515665796376</v>
       </c>
       <c r="D73">
         <v>0.6691945287461464</v>
@@ -2074,10 +2293,13 @@
         <v>0.6136964572397244</v>
       </c>
       <c r="G73">
+        <v>0.4753228577439089</v>
+      </c>
+      <c r="H73">
         <v>0.6057118133853626</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:8">
       <c r="A74">
         <v>0.662278742</v>
       </c>
@@ -2085,7 +2307,7 @@
         <v>0.5709598268950711</v>
       </c>
       <c r="C74">
-        <v>0.6315903449738371</v>
+        <v>0.4402191333173687</v>
       </c>
       <c r="D74">
         <v>0.6910484366983278</v>
@@ -2097,10 +2319,13 @@
         <v>0.6360395122491987</v>
       </c>
       <c r="G74">
+        <v>0.4926084802327408</v>
+      </c>
+      <c r="H74">
         <v>0.6283433650197774</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:8">
       <c r="A75">
         <v>0.456505507</v>
       </c>
@@ -2108,7 +2333,7 @@
         <v>0.3184086813803343</v>
       </c>
       <c r="C75">
-        <v>0.3331876308010954</v>
+        <v>0.2231000148386561</v>
       </c>
       <c r="D75">
         <v>0.3737688271924748</v>
@@ -2120,10 +2345,13 @@
         <v>0.3332176105236787</v>
       </c>
       <c r="G75">
+        <v>0.2529337426689746</v>
+      </c>
+      <c r="H75">
         <v>0.3285343872396782</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:8">
       <c r="A76">
         <v>-0.181605646</v>
       </c>
@@ -2131,7 +2359,7 @@
         <v>-0.1848648973891894</v>
       </c>
       <c r="C76">
-        <v>-0.1694172321821299</v>
+        <v>-0.2542127448579455</v>
       </c>
       <c r="D76">
         <v>-0.2166328660303428</v>
@@ -2143,10 +2371,13 @@
         <v>-0.1722907951667788</v>
       </c>
       <c r="G76">
+        <v>-0.1448218207166277</v>
+      </c>
+      <c r="H76">
         <v>-0.1687903262635242</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:8">
       <c r="A77">
         <v>0.647849754</v>
       </c>
@@ -2154,7 +2385,7 @@
         <v>0.4215079526921449</v>
       </c>
       <c r="C77">
-        <v>0.4307521607645295</v>
+        <v>0.3821022339467148</v>
       </c>
       <c r="D77">
         <v>0.4560940523201704</v>
@@ -2166,10 +2397,13 @@
         <v>0.4292307812336733</v>
       </c>
       <c r="G77">
+        <v>0.3299029233207444</v>
+      </c>
+      <c r="H77">
         <v>0.424474419665595</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:8">
       <c r="A78">
         <v>-0.151031448</v>
       </c>
@@ -2177,7 +2411,7 @@
         <v>-0.4414734802421283</v>
       </c>
       <c r="C78">
-        <v>-0.4478381464343915</v>
+        <v>-0.4539159640885037</v>
       </c>
       <c r="D78">
         <v>-0.4402231794753995</v>
@@ -2189,10 +2423,13 @@
         <v>-0.4415890532265882</v>
       </c>
       <c r="G78">
+        <v>-0.3650198219621916</v>
+      </c>
+      <c r="H78">
         <v>-0.4486778761222822</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:8">
       <c r="A79">
         <v>0.204622557</v>
       </c>
@@ -2200,7 +2437,7 @@
         <v>-0.03954956793619075</v>
       </c>
       <c r="C79">
-        <v>-0.01579833827254072</v>
+        <v>-0.04297178762303158</v>
       </c>
       <c r="D79">
         <v>0.001458433699311923</v>
@@ -2212,10 +2449,13 @@
         <v>-0.01887096344476689</v>
       </c>
       <c r="G79">
+        <v>-0.02373564599302212</v>
+      </c>
+      <c r="H79">
         <v>-0.02050156642427843</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:8">
       <c r="A80">
         <v>0.6727765610000001</v>
       </c>
@@ -2223,7 +2463,7 @@
         <v>0.5560464449135224</v>
       </c>
       <c r="C80">
-        <v>0.6183756758666743</v>
+        <v>0.5260518003706547</v>
       </c>
       <c r="D80">
         <v>0.5769013195779183</v>
@@ -2235,10 +2475,13 @@
         <v>0.6133098560726664</v>
       </c>
       <c r="G80">
+        <v>0.4728269469209006</v>
+      </c>
+      <c r="H80">
         <v>0.6072452856613031</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:8">
       <c r="A81">
         <v>1.409854459</v>
       </c>
@@ -2246,7 +2489,7 @@
         <v>1.23864835846565</v>
       </c>
       <c r="C81">
-        <v>1.309459077751803</v>
+        <v>1.186063852404969</v>
       </c>
       <c r="D81">
         <v>1.268139749407179</v>
@@ -2258,10 +2501,13 @@
         <v>1.304941081642034</v>
       </c>
       <c r="G81">
+        <v>1.018401395288801</v>
+      </c>
+      <c r="H81">
         <v>1.2927682541263</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:8">
       <c r="A82">
         <v>1.436857019</v>
       </c>
@@ -2269,7 +2515,7 @@
         <v>1.189181054470793</v>
       </c>
       <c r="C82">
-        <v>1.220420741266864</v>
+        <v>1.158222768051846</v>
       </c>
       <c r="D82">
         <v>1.146322447387556</v>
@@ -2281,10 +2527,13 @@
         <v>1.21188961073329</v>
       </c>
       <c r="G82">
+        <v>0.9460113031204238</v>
+      </c>
+      <c r="H82">
         <v>1.201015595770309</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:8">
       <c r="A83">
         <v>-0.078187413</v>
       </c>
@@ -2292,7 +2541,7 @@
         <v>-0.4777878517646848</v>
       </c>
       <c r="C83">
-        <v>-0.3937493332930366</v>
+        <v>-0.4240857114721407</v>
       </c>
       <c r="D83">
         <v>-0.4551802763625509</v>
@@ -2304,10 +2553,13 @@
         <v>-0.3731231704237526</v>
       </c>
       <c r="G83">
+        <v>-0.3172656731251585</v>
+      </c>
+      <c r="H83">
         <v>-0.3858372622832756</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:8">
       <c r="A84">
         <v>-0.089819775</v>
       </c>
@@ -2315,7 +2567,7 @@
         <v>-0.3142111532803021</v>
       </c>
       <c r="C84">
-        <v>-0.2037499776339326</v>
+        <v>-0.2379636208207484</v>
       </c>
       <c r="D84">
         <v>-0.2730224857991948</v>
@@ -2327,10 +2579,13 @@
         <v>-0.1997308235287824</v>
       </c>
       <c r="G84">
+        <v>-0.1700299084920769</v>
+      </c>
+      <c r="H84">
         <v>-0.2008598702266237</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:8">
       <c r="A85">
         <v>-0.951749297</v>
       </c>
@@ -2338,7 +2593,7 @@
         <v>-1.052109682200372</v>
       </c>
       <c r="C85">
-        <v>-0.9116751296343498</v>
+        <v>-0.94237377311923</v>
       </c>
       <c r="D85">
         <v>-0.9689286909440492</v>
@@ -2350,10 +2605,13 @@
         <v>-0.8910776382232894</v>
       </c>
       <c r="G85">
+        <v>-0.7215741793285488</v>
+      </c>
+      <c r="H85">
         <v>-0.8922280012728956</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:8">
       <c r="A86">
         <v>-0.611776729</v>
       </c>
@@ -2361,7 +2619,7 @@
         <v>-0.5152780755148332</v>
       </c>
       <c r="C86">
-        <v>-0.379342278268806</v>
+        <v>-0.3944196230730213</v>
       </c>
       <c r="D86">
         <v>-0.4344840166016919</v>
@@ -2373,10 +2631,13 @@
         <v>-0.3747944485169569</v>
       </c>
       <c r="G86">
+        <v>-0.3180664125063943</v>
+      </c>
+      <c r="H86">
         <v>-0.3738892762197526</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:8">
       <c r="A87">
         <v>-1.503113365</v>
       </c>
@@ -2384,7 +2645,7 @@
         <v>-1.586393333853157</v>
       </c>
       <c r="C87">
-        <v>-1.483702408555807</v>
+        <v>-1.44568318440334</v>
       </c>
       <c r="D87">
         <v>-1.493599820027991</v>
@@ -2396,10 +2657,13 @@
         <v>-1.434412160399382</v>
       </c>
       <c r="G87">
+        <v>-1.169097039252953</v>
+      </c>
+      <c r="H87">
         <v>-1.451950752862983</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:8">
       <c r="A88">
         <v>-0.95035541</v>
       </c>
@@ -2407,7 +2671,7 @@
         <v>-1.359712416482687</v>
       </c>
       <c r="C88">
-        <v>-1.270249079454969</v>
+        <v>-1.197841795561652</v>
       </c>
       <c r="D88">
         <v>-1.262364017558427</v>
@@ -2419,10 +2683,13 @@
         <v>-1.247702933521181</v>
       </c>
       <c r="G88">
+        <v>-1.007531933150079</v>
+      </c>
+      <c r="H88">
         <v>-1.246812125971354</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:8">
       <c r="A89">
         <v>-0.869041164</v>
       </c>
@@ -2430,7 +2697,7 @@
         <v>-0.7851434786380161</v>
       </c>
       <c r="C89">
-        <v>-0.6996496377077648</v>
+        <v>-0.7035395158885788</v>
       </c>
       <c r="D89">
         <v>-0.7337465210500311</v>
@@ -2442,10 +2709,13 @@
         <v>-0.6836549406256648</v>
       </c>
       <c r="G89">
+        <v>-0.5599508801317106</v>
+      </c>
+      <c r="H89">
         <v>-0.6883184398707081</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:8">
       <c r="A90">
         <v>-0.621619324</v>
       </c>
@@ -2453,7 +2723,7 @@
         <v>-0.6771285866481079</v>
       </c>
       <c r="C90">
-        <v>-0.5897337828728689</v>
+        <v>-0.604558636332906</v>
       </c>
       <c r="D90">
         <v>-0.6373983816269089</v>
@@ -2465,10 +2735,13 @@
         <v>-0.5316621946674033</v>
       </c>
       <c r="G90">
+        <v>-0.4737405569829399</v>
+      </c>
+      <c r="H90">
         <v>-0.5788725544091109</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:8">
       <c r="A91">
         <v>0.820733698</v>
       </c>
@@ -2476,7 +2749,7 @@
         <v>0.2857775914272223</v>
       </c>
       <c r="C91">
-        <v>0.3597080126085314</v>
+        <v>0.3141998902350692</v>
       </c>
       <c r="D91">
         <v>0.2918760664523546</v>
@@ -2488,10 +2761,13 @@
         <v>0.3559721696032044</v>
       </c>
       <c r="G91">
+        <v>0.2692726176179518</v>
+      </c>
+      <c r="H91">
         <v>0.3518402864698747</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:8">
       <c r="A92">
         <v>1.157975086</v>
       </c>
@@ -2499,7 +2775,7 @@
         <v>0.6004952847976842</v>
       </c>
       <c r="C92">
-        <v>0.6605940568690289</v>
+        <v>0.6092327291149681</v>
       </c>
       <c r="D92">
         <v>0.5790859942584703</v>
@@ -2511,10 +2787,13 @@
         <v>0.6546266269577329</v>
       </c>
       <c r="G92">
+        <v>0.5047737920853327</v>
+      </c>
+      <c r="H92">
         <v>0.6485131042535994</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:8">
       <c r="A93">
         <v>1.16180901</v>
       </c>
@@ -2522,7 +2801,7 @@
         <v>0.629473412497797</v>
       </c>
       <c r="C93">
-        <v>0.6905522249364631</v>
+        <v>0.6342837282322814</v>
       </c>
       <c r="D93">
         <v>0.6045694025600047</v>
@@ -2534,10 +2813,13 @@
         <v>0.6839090801606325</v>
       </c>
       <c r="G93">
+        <v>0.5282049753300156</v>
+      </c>
+      <c r="H93">
         <v>0.6775688252224931</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:8">
       <c r="A94">
         <v>0.673844651</v>
       </c>
@@ -2545,7 +2827,7 @@
         <v>0.3754932513998903</v>
       </c>
       <c r="C94">
-        <v>0.4388537506141158</v>
+        <v>0.3972468181901891</v>
       </c>
       <c r="D94">
         <v>0.3679879864136921</v>
@@ -2557,10 +2839,13 @@
         <v>0.4340509326837016</v>
       </c>
       <c r="G94">
+        <v>0.3312873412604576</v>
+      </c>
+      <c r="H94">
         <v>0.4295305223754062</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:8">
       <c r="A95">
         <v>0.576154411</v>
       </c>
@@ -2568,7 +2853,7 @@
         <v>0.1903608953149541</v>
       </c>
       <c r="C95">
-        <v>0.2715405943125805</v>
+        <v>0.2300847270267722</v>
       </c>
       <c r="D95">
         <v>0.1996166016697674</v>
@@ -2580,10 +2865,13 @@
         <v>0.2688952583788535</v>
       </c>
       <c r="G95">
+        <v>0.2003212755156965</v>
+      </c>
+      <c r="H95">
         <v>0.2652903133908052</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:8">
       <c r="A96">
         <v>-0.247999935</v>
       </c>
@@ -2591,7 +2879,7 @@
         <v>-0.4680051071522791</v>
       </c>
       <c r="C96">
-        <v>-0.3558827373759933</v>
+        <v>-0.3887659360503674</v>
       </c>
       <c r="D96">
         <v>-0.4225844268174876</v>
@@ -2603,10 +2891,13 @@
         <v>-0.3483573783984094</v>
       </c>
       <c r="G96">
+        <v>-0.2856055159137933</v>
+      </c>
+      <c r="H96">
         <v>-0.3495233878854893</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:8">
       <c r="A97">
         <v>-1.022406207</v>
       </c>
@@ -2614,7 +2905,7 @@
         <v>-1.262701313287432</v>
       </c>
       <c r="C97">
-        <v>-1.121134306539448</v>
+        <v>-1.152562578171491</v>
       </c>
       <c r="D97">
         <v>-1.174168600565034</v>
@@ -2626,10 +2917,13 @@
         <v>-1.086811412954209</v>
       </c>
       <c r="G97">
+        <v>-0.8836407746044924</v>
+      </c>
+      <c r="H97">
         <v>-1.095741797929685</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:8">
       <c r="A98">
         <v>-0.898568511</v>
       </c>
@@ -2637,7 +2931,7 @@
         <v>-0.9033686851803443</v>
       </c>
       <c r="C98">
-        <v>-0.758625031453422</v>
+        <v>-0.7668632560477872</v>
       </c>
       <c r="D98">
         <v>-0.8078951553862713</v>
@@ -2649,10 +2943,13 @@
         <v>-0.7460759561250787</v>
       </c>
       <c r="G98">
+        <v>-0.6040000182024874</v>
+      </c>
+      <c r="H98">
         <v>-0.7440330483802021</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:8">
       <c r="A99">
         <v>-0.35746994</v>
       </c>
@@ -2660,7 +2957,7 @@
         <v>-0.2817707184184445</v>
       </c>
       <c r="C99">
-        <v>-0.1733991372653879</v>
+        <v>-0.1880979766555269</v>
       </c>
       <c r="D99">
         <v>-0.2144451955589171</v>
@@ -2672,10 +2969,13 @@
         <v>-0.1730317151739461</v>
       </c>
       <c r="G99">
+        <v>-0.1482374843056306</v>
+      </c>
+      <c r="H99">
         <v>-0.1733491934187259</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:8">
       <c r="A100">
         <v>-0.676801503</v>
       </c>
@@ -2683,7 +2983,7 @@
         <v>-0.03589502664881495</v>
       </c>
       <c r="C100">
-        <v>0.05942264183526662</v>
+        <v>0.04701752319563251</v>
       </c>
       <c r="D100">
         <v>0.02956448087250192</v>
@@ -2695,10 +2995,13 @@
         <v>0.05773666950914638</v>
       </c>
       <c r="G100">
+        <v>0.03301273304825333</v>
+      </c>
+      <c r="H100">
         <v>0.05590387138217869</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:8">
       <c r="A101">
         <v>-0.963128334</v>
       </c>
@@ -2706,7 +3009,7 @@
         <v>-0.2714813996923306</v>
       </c>
       <c r="C101">
-        <v>-0.1862343568994309</v>
+        <v>-0.2040609452420336</v>
       </c>
       <c r="D101">
         <v>-0.2274014537221751</v>
@@ -2718,10 +3021,13 @@
         <v>-0.1846713402652682</v>
       </c>
       <c r="G101">
+        <v>-0.1583010320386279</v>
+      </c>
+      <c r="H101">
         <v>-0.1857110303861134</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:8">
       <c r="A102">
         <v>-1.089650457</v>
       </c>
@@ -2729,7 +3035,7 @@
         <v>-0.543310711331521</v>
       </c>
       <c r="C102">
-        <v>-0.4559610482209983</v>
+        <v>-0.4714980848690992</v>
       </c>
       <c r="D102">
         <v>-0.5055170572922909</v>
@@ -2741,10 +3047,13 @@
         <v>-0.4386964008233007</v>
       </c>
       <c r="G102">
+        <v>-0.3548721287588452</v>
+      </c>
+      <c r="H102">
         <v>-0.4482396553469484</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:8">
       <c r="A103">
         <v>-1.754660522</v>
       </c>
@@ -2752,7 +3061,7 @@
         <v>-1.119628518689733</v>
       </c>
       <c r="C103">
-        <v>-1.043900961581805</v>
+        <v>-1.079399188797008</v>
       </c>
       <c r="D103">
         <v>-1.089818105777498</v>
@@ -2764,10 +3073,13 @@
         <v>-1.036630924677298</v>
       </c>
       <c r="G103">
+        <v>-0.8246280265794812</v>
+      </c>
+      <c r="H103">
         <v>-1.020901351224637</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:8">
       <c r="A104">
         <v>-1.724252511</v>
       </c>
@@ -2775,7 +3087,7 @@
         <v>-1.679550443666403</v>
       </c>
       <c r="C104">
-        <v>-1.617336650393944</v>
+        <v>-1.670710116794829</v>
       </c>
       <c r="D104">
         <v>-1.656937217935285</v>
@@ -2787,10 +3099,13 @@
         <v>-1.594963767926163</v>
       </c>
       <c r="G104">
+        <v>-1.265988858871832</v>
+      </c>
+      <c r="H104">
         <v>-1.57509099895009</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:8">
       <c r="A105">
         <v>-1.868408762</v>
       </c>
@@ -2798,7 +3113,7 @@
         <v>-1.900088281981663</v>
       </c>
       <c r="C105">
-        <v>-1.850188140817828</v>
+        <v>-1.889383449106632</v>
       </c>
       <c r="D105">
         <v>-1.885612660697728</v>
@@ -2810,10 +3125,13 @@
         <v>-1.818030661244866</v>
       </c>
       <c r="G105">
+        <v>-1.442308010068137</v>
+      </c>
+      <c r="H105">
         <v>-1.795288931054512</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:8">
       <c r="A106">
         <v>-0.07703964000000001</v>
       </c>
@@ -2821,7 +3139,7 @@
         <v>-0.5157162875729899</v>
       </c>
       <c r="C106">
-        <v>-0.4411523899697865</v>
+        <v>-0.4688772645966801</v>
       </c>
       <c r="D106">
         <v>-0.5000012488311479</v>
@@ -2833,10 +3151,13 @@
         <v>-0.4511678314581786</v>
       </c>
       <c r="G106">
+        <v>-0.3528622985445702</v>
+      </c>
+      <c r="H106">
         <v>-0.4323969088358427</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:8">
       <c r="A107">
         <v>-0.058419279</v>
       </c>
@@ -2844,7 +3165,7 @@
         <v>-0.6100463556619444</v>
       </c>
       <c r="C107">
-        <v>-0.5280004544099512</v>
+        <v>-0.5569605901892003</v>
       </c>
       <c r="D107">
         <v>-0.5867356830938075</v>
@@ -2856,10 +3177,13 @@
         <v>-0.4196810747657454</v>
       </c>
       <c r="G107">
+        <v>-0.4359985582859557</v>
+      </c>
+      <c r="H107">
         <v>-0.5167799696232488</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:8">
       <c r="A108">
         <v>1.204247991</v>
       </c>
@@ -2867,7 +3191,7 @@
         <v>0.6383069973262471</v>
       </c>
       <c r="C108">
-        <v>0.71697146473115</v>
+        <v>0.670964099433689</v>
       </c>
       <c r="D108">
         <v>0.6370132703027548</v>
@@ -2879,10 +3203,13 @@
         <v>0.7099351838015669</v>
       </c>
       <c r="G108">
+        <v>0.5493178373182108</v>
+      </c>
+      <c r="H108">
         <v>0.7029461303229808</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:8">
       <c r="A109">
         <v>1.183657404</v>
       </c>
@@ -2890,7 +3217,7 @@
         <v>1.27182399939069</v>
       </c>
       <c r="C109">
-        <v>1.326554891581208</v>
+        <v>1.27107763592263</v>
       </c>
       <c r="D109">
         <v>1.254257614043573</v>
@@ -2902,10 +3229,13 @@
         <v>1.319014200107225</v>
       </c>
       <c r="G109">
+        <v>1.029965781084555</v>
+      </c>
+      <c r="H109">
         <v>1.306424786589029</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:8">
       <c r="A110">
         <v>1.235714724</v>
       </c>
@@ -2913,7 +3243,7 @@
         <v>1.541249141671778</v>
       </c>
       <c r="C110">
-        <v>1.581165568370438</v>
+        <v>1.532453182851149</v>
       </c>
       <c r="D110">
         <v>1.524879670383841</v>
@@ -2925,10 +3255,13 @@
         <v>1.576584355991212</v>
       </c>
       <c r="G110">
+        <v>1.233413567516884</v>
+      </c>
+      <c r="H110">
         <v>1.561466532206047</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:8">
       <c r="A111">
         <v>1.193822144</v>
       </c>
@@ -2936,7 +3269,7 @@
         <v>1.004832013624319</v>
       </c>
       <c r="C111">
-        <v>1.085424359096062</v>
+        <v>1.017005830449726</v>
       </c>
       <c r="D111">
         <v>1.04681169672663</v>
@@ -2948,10 +3281,13 @@
         <v>1.081047867691634</v>
       </c>
       <c r="G111">
+        <v>0.8422006710794817</v>
+      </c>
+      <c r="H111">
         <v>1.070462357024889</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:8">
       <c r="A112">
         <v>1.680661976</v>
       </c>
@@ -2959,7 +3295,7 @@
         <v>1.503607973815888</v>
       </c>
       <c r="C112">
-        <v>1.574261917368666</v>
+        <v>1.498699717029012</v>
       </c>
       <c r="D112">
         <v>1.54569575852202</v>
@@ -2971,10 +3307,13 @@
         <v>1.572619792555156</v>
       </c>
       <c r="G112">
+        <v>1.229403903045808</v>
+      </c>
+      <c r="H112">
         <v>1.557871753086343</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:8">
       <c r="A113">
         <v>1.735508276</v>
       </c>
@@ -2982,7 +3321,7 @@
         <v>1.715104648449981</v>
       </c>
       <c r="C113">
-        <v>1.771628490657847</v>
+        <v>1.708990806705642</v>
       </c>
       <c r="D113">
         <v>1.749247930263758</v>
@@ -2994,10 +3333,13 @@
         <v>1.772506199430236</v>
       </c>
       <c r="G113">
+        <v>1.387311155398386</v>
+      </c>
+      <c r="H113">
         <v>1.755867534524208</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:8">
       <c r="A114">
         <v>1.120645867</v>
       </c>
@@ -3005,7 +3347,7 @@
         <v>1.612899740362318</v>
       </c>
       <c r="C114">
-        <v>1.66923596493311</v>
+        <v>1.598310523517529</v>
       </c>
       <c r="D114">
         <v>1.623294584684302</v>
@@ -3017,10 +3359,13 @@
         <v>1.665824475109505</v>
       </c>
       <c r="G114">
+        <v>1.302992343689792</v>
+      </c>
+      <c r="H114">
         <v>1.650250926654327</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:8">
       <c r="A115">
         <v>0.220765723</v>
       </c>
@@ -3028,7 +3373,7 @@
         <v>0.4721540703437359</v>
       </c>
       <c r="C115">
-        <v>0.5431417288501725</v>
+        <v>0.4901714863019302</v>
       </c>
       <c r="D115">
         <v>0.4740264926270099</v>
@@ -3040,10 +3385,13 @@
         <v>0.5378167295075758</v>
       </c>
       <c r="G115">
+        <v>0.4130265127569201</v>
+      </c>
+      <c r="H115">
         <v>0.532409634550592</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:8">
       <c r="A116">
         <v>0.291028273</v>
       </c>
@@ -3051,7 +3399,7 @@
         <v>0.382367846848612</v>
       </c>
       <c r="C116">
-        <v>0.4475071809273498</v>
+        <v>0.4014494362293998</v>
       </c>
       <c r="D116">
         <v>0.3678423104602295</v>
@@ -3063,10 +3411,13 @@
         <v>0.4436624776408306</v>
       </c>
       <c r="G116">
+        <v>0.337981045167287</v>
+      </c>
+      <c r="H116">
         <v>0.4389212364542825</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:8">
       <c r="A117">
         <v>0.583045483</v>
       </c>
@@ -3074,7 +3425,7 @@
         <v>1.120466296853424</v>
       </c>
       <c r="C117">
-        <v>1.164538286849639</v>
+        <v>1.095855127207737</v>
       </c>
       <c r="D117">
         <v>1.077004408046796</v>
@@ -3086,10 +3437,13 @@
         <v>1.155296343135262</v>
       </c>
       <c r="G117">
+        <v>0.9003645440859769</v>
+      </c>
+      <c r="H117">
         <v>1.144955285247555</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:8">
       <c r="A118">
         <v>1.459657324</v>
       </c>
@@ -3097,7 +3451,7 @@
         <v>1.522327791668313</v>
       </c>
       <c r="C118">
-        <v>1.535171145107328</v>
+        <v>1.470100972514778</v>
       </c>
       <c r="D118">
         <v>1.461668448373782</v>
@@ -3109,10 +3463,13 @@
         <v>1.527190341573646</v>
       </c>
       <c r="G118">
+        <v>1.194868087357831</v>
+      </c>
+      <c r="H118">
         <v>1.513338067323604</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:8">
       <c r="A119">
         <v>0.957846139</v>
       </c>
@@ -3120,7 +3477,7 @@
         <v>1.302945303299518</v>
       </c>
       <c r="C119">
-        <v>1.33751821406895</v>
+        <v>1.282211940841947</v>
       </c>
       <c r="D119">
         <v>1.258422139094671</v>
@@ -3132,10 +3489,13 @@
         <v>1.328878092099837</v>
       </c>
       <c r="G119">
+        <v>1.037918763551051</v>
+      </c>
+      <c r="H119">
         <v>1.316565082762714</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:8">
       <c r="A120">
         <v>1.102629823</v>
       </c>
@@ -3143,7 +3503,7 @@
         <v>0.437826648007514</v>
       </c>
       <c r="C120">
-        <v>0.5260979649925716</v>
+        <v>0.4821339121564043</v>
       </c>
       <c r="D120">
         <v>0.4476738288747563</v>
@@ -3155,10 +3515,13 @@
         <v>0.5204185360319896</v>
       </c>
       <c r="G120">
+        <v>0.3996145425387881</v>
+      </c>
+      <c r="H120">
         <v>0.5149967946893451</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:8">
       <c r="A121">
         <v>1.64061108</v>
       </c>
@@ -3166,7 +3529,7 @@
         <v>1.401880230335193</v>
       </c>
       <c r="C121">
-        <v>1.448562830913245</v>
+        <v>1.396355860967681</v>
       </c>
       <c r="D121">
         <v>1.376973507754879</v>
@@ -3178,10 +3541,13 @@
         <v>1.441297528618942</v>
       </c>
       <c r="G121">
+        <v>1.126440455969221</v>
+      </c>
+      <c r="H121">
         <v>1.427582957659017</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:8">
       <c r="A122">
         <v>1.886908677</v>
       </c>
@@ -3189,7 +3555,7 @@
         <v>1.473087447377131</v>
       </c>
       <c r="C122">
-        <v>1.517257234617941</v>
+        <v>1.466336674727188</v>
       </c>
       <c r="D122">
         <v>1.460269506761795</v>
@@ -3201,10 +3567,13 @@
         <v>1.512284530328691</v>
       </c>
       <c r="G122">
+        <v>1.182676435951261</v>
+      </c>
+      <c r="H122">
         <v>1.497768789223592</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:8">
       <c r="A123">
         <v>1.733513011</v>
       </c>
@@ -3212,7 +3581,7 @@
         <v>1.826815652772518</v>
       </c>
       <c r="C123">
-        <v>1.8864131121447</v>
+        <v>1.835845337008773</v>
       </c>
       <c r="D123">
         <v>1.862104331720682</v>
@@ -3224,10 +3593,13 @@
         <v>1.888976518151738</v>
       </c>
       <c r="G123">
+        <v>1.479536336917554</v>
+      </c>
+      <c r="H123">
         <v>1.870819604390712</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:8">
       <c r="A124">
         <v>-0.0362457</v>
       </c>
@@ -3235,7 +3607,7 @@
         <v>0.3777556703659038</v>
       </c>
       <c r="C124">
-        <v>0.4680064950747977</v>
+        <v>0.431917010424876</v>
       </c>
       <c r="D124">
         <v>0.4347221351963342</v>
@@ -3247,10 +3619,13 @@
         <v>0.4638640232145162</v>
       </c>
       <c r="G124">
+        <v>0.3541682331259755</v>
+      </c>
+      <c r="H124">
         <v>0.4589387283965907</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:8">
       <c r="A125">
         <v>0.430903942</v>
       </c>
@@ -3258,7 +3633,7 @@
         <v>0.8439876171520723</v>
       </c>
       <c r="C125">
-        <v>0.9137206144155456</v>
+        <v>0.8548356020599764</v>
       </c>
       <c r="D125">
         <v>0.875361617221756</v>
@@ -3270,10 +3645,13 @@
         <v>0.9087208210008961</v>
       </c>
       <c r="G125">
+        <v>0.7059931931230338</v>
+      </c>
+      <c r="H125">
         <v>0.8999921090239236</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:8">
       <c r="A126">
         <v>-0.243546309</v>
       </c>
@@ -3281,7 +3659,7 @@
         <v>-0.07583556108168893</v>
       </c>
       <c r="C126">
-        <v>0.008616048410380824</v>
+        <v>-0.01469599923261868</v>
       </c>
       <c r="D126">
         <v>-0.04542667808157531</v>
@@ -3293,10 +3671,13 @@
         <v>0.008981782974863226</v>
       </c>
       <c r="G126">
+        <v>-0.00562655369143001</v>
+      </c>
+      <c r="H126">
         <v>0.006720923291283258</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:8">
       <c r="A127">
         <v>-0.931687809</v>
       </c>
@@ -3304,7 +3685,7 @@
         <v>-0.9851676287888931</v>
       </c>
       <c r="C127">
-        <v>-0.9075512053119118</v>
+        <v>-0.9414451520797851</v>
       </c>
       <c r="D127">
         <v>-0.9565929258235214</v>
@@ -3316,10 +3697,13 @@
         <v>-0.9032943608816181</v>
       </c>
       <c r="G127">
+        <v>-0.7189888868659484</v>
+      </c>
+      <c r="H127">
         <v>-0.8882266027272993</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:8">
       <c r="A128">
         <v>0.141116369</v>
       </c>
@@ -3327,7 +3711,7 @@
         <v>0.07314062434255175</v>
       </c>
       <c r="C128">
-        <v>0.1440938786723752</v>
+        <v>0.1035163211325546</v>
       </c>
       <c r="D128">
         <v>0.06775236283344864</v>
@@ -3339,10 +3723,13 @@
         <v>0.145424698743702</v>
       </c>
       <c r="G128">
+        <v>0.1009723658557258</v>
+      </c>
+      <c r="H128">
         <v>0.1410596719559379</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:8">
       <c r="A129">
         <v>0.56391939</v>
       </c>
@@ -3350,7 +3737,7 @@
         <v>0.5176311989286843</v>
       </c>
       <c r="C129">
-        <v>0.5819502405172543</v>
+        <v>0.5286869928115587</v>
       </c>
       <c r="D129">
         <v>0.4966474744787379</v>
@@ -3362,10 +3749,13 @@
         <v>0.5763044973788268</v>
       </c>
       <c r="G129">
+        <v>0.4431557693258218</v>
+      </c>
+      <c r="H129">
         <v>0.5707559490502738</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:8">
       <c r="A130">
         <v>1.941603295</v>
       </c>
@@ -3373,7 +3763,7 @@
         <v>1.797427546851027</v>
       </c>
       <c r="C130">
-        <v>1.792946946769245</v>
+        <v>1.731350503908423</v>
       </c>
       <c r="D130">
         <v>1.720727418398734</v>
@@ -3385,10 +3775,13 @@
         <v>1.786186129971514</v>
       </c>
       <c r="G130">
+        <v>1.399237756119171</v>
+      </c>
+      <c r="H130">
         <v>1.769833694971257</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:8">
       <c r="A131">
         <v>0.686945786</v>
       </c>
@@ -3396,7 +3789,7 @@
         <v>0.7600987933114342</v>
       </c>
       <c r="C131">
-        <v>0.8234382753747083</v>
+        <v>0.7702607538387449</v>
       </c>
       <c r="D131">
         <v>0.7463440552796954</v>
@@ -3408,10 +3801,13 @@
         <v>0.8160121349024346</v>
       </c>
       <c r="G131">
+        <v>0.6329724541894964</v>
+      </c>
+      <c r="H131">
         <v>0.8083261992011982</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:8">
       <c r="A132">
         <v>0.489776809</v>
       </c>
@@ -3419,7 +3815,7 @@
         <v>1.109625556100302</v>
       </c>
       <c r="C132">
-        <v>1.160032734242288</v>
+        <v>1.115071889425367</v>
       </c>
       <c r="D132">
         <v>1.077871908694356</v>
@@ -3431,10 +3827,13 @@
         <v>1.151298376404528</v>
       </c>
       <c r="G132">
+        <v>0.8977815623971448</v>
+      </c>
+      <c r="H132">
         <v>1.140414037417551</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:8">
       <c r="A133">
         <v>-0.927615797</v>
       </c>
@@ -3442,7 +3841,7 @@
         <v>0.006553851352811211</v>
       </c>
       <c r="C133">
-        <v>0.1228675377773724</v>
+        <v>0.08171597684289134</v>
       </c>
       <c r="D133">
         <v>0.05196028601724384</v>
@@ -3454,10 +3853,13 @@
         <v>0.1208631025061702</v>
       </c>
       <c r="G133">
+        <v>0.08414120428656713</v>
+      </c>
+      <c r="H133">
         <v>0.1184653142487875</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:8">
       <c r="A134">
         <v>-0.570785532</v>
       </c>
@@ -3465,7 +3867,7 @@
         <v>-0.0008408127219168221</v>
       </c>
       <c r="C134">
-        <v>0.1181385917195056</v>
+        <v>0.0893077460374897</v>
       </c>
       <c r="D134">
         <v>0.05816426765575701</v>
@@ -3477,10 +3879,13 @@
         <v>0.1159551334510149</v>
       </c>
       <c r="G134">
+        <v>0.08020454102259109</v>
+      </c>
+      <c r="H134">
         <v>0.1136374006455805</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:8">
       <c r="A135">
         <v>0.629936161</v>
       </c>
@@ -3488,7 +3893,7 @@
         <v>0.16030704481354</v>
       </c>
       <c r="C135">
-        <v>0.2608445832555576</v>
+        <v>0.2268641974305579</v>
       </c>
       <c r="D135">
         <v>0.2175882917393073</v>
@@ -3500,10 +3905,13 @@
         <v>0.2572734092808652</v>
       </c>
       <c r="G135">
+        <v>0.1918020680137833</v>
+      </c>
+      <c r="H135">
         <v>0.2538543684656951</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:8">
       <c r="A136">
         <v>1.229927464</v>
       </c>
@@ -3511,7 +3919,7 @@
         <v>1.037002178700838</v>
       </c>
       <c r="C136">
-        <v>1.116249326818573</v>
+        <v>1.048052165382298</v>
       </c>
       <c r="D136">
         <v>1.083485896291404</v>
@@ -3523,10 +3931,13 @@
         <v>1.112011329633981</v>
       </c>
       <c r="G136">
+        <v>0.865981386611014</v>
+      </c>
+      <c r="H136">
         <v>1.101484204208662</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:8">
       <c r="A137">
         <v>0.831135585</v>
       </c>
@@ -3534,7 +3945,7 @@
         <v>0.5537135771143457</v>
       </c>
       <c r="C137">
-        <v>0.628261394586705</v>
+        <v>0.5804308914461327</v>
       </c>
       <c r="D137">
         <v>0.5871086969373068</v>
@@ -3546,10 +3957,13 @@
         <v>0.6232830322767642</v>
       </c>
       <c r="G137">
+        <v>0.4806837951120471</v>
+      </c>
+      <c r="H137">
         <v>0.6170058868841531</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:8">
       <c r="A138">
         <v>-0.615633494</v>
       </c>
@@ -3557,7 +3971,7 @@
         <v>-0.2884491024204741</v>
       </c>
       <c r="C138">
-        <v>-0.2022115984638043</v>
+        <v>-0.2208719875443874</v>
       </c>
       <c r="D138">
         <v>-0.2546112764088382</v>
@@ -3569,10 +3983,13 @@
         <v>-0.197541417956839</v>
       </c>
       <c r="G138">
+        <v>-0.1700519042365051</v>
+      </c>
+      <c r="H138">
         <v>-0.1999935406353587</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:8">
       <c r="A139">
         <v>-0.504548817</v>
       </c>
@@ -3580,7 +3997,7 @@
         <v>-0.5635677100580835</v>
       </c>
       <c r="C139">
-        <v>-0.4833372475310305</v>
+        <v>-0.5137861855303244</v>
       </c>
       <c r="D139">
         <v>-0.5406772280575195</v>
@@ -3592,6 +4009,9 @@
         <v>-0.4980046295116665</v>
       </c>
       <c r="G139">
+        <v>-0.3917262897718338</v>
+      </c>
+      <c r="H139">
         <v>-0.4745315790489228</v>
       </c>
     </row>

</xml_diff>

<commit_message>
goliatt ter 18 fev 2025 23:33:47 -03
</commit_message>
<xml_diff>
--- a/table_best_models____spi-3__test.xlsx
+++ b/table_best_models____spi-3__test.xlsx
@@ -19,22 +19,22 @@
     <t>Observed</t>
   </si>
   <si>
-    <t>Lasso ($\beta = $0.0) ($\beta = $0.0)</t>
+    <t>Lasso ($\beta = $0.0)</t>
   </si>
   <si>
-    <t>Lasso ($\beta = $0.1) ($\beta = $0.1)</t>
+    <t>Lasso ($\beta = $0.1)</t>
   </si>
   <si>
-    <t>Lasso ($\beta = $0.5) ($\beta = $0.5)</t>
+    <t>Lasso ($\beta = $0.5)</t>
   </si>
   <si>
-    <t>Lasso ($\beta = $1.0) ($\beta = $1.0)</t>
+    <t>Lasso ($\beta = $1.0)</t>
   </si>
   <si>
-    <t>Lasso ($\beta = $1.5) ($\beta = $1.5)</t>
+    <t>Lasso ($\beta = $1.5)</t>
   </si>
   <si>
-    <t>Lasso ($\beta = $2.0) ($\beta = $2.0)</t>
+    <t>Lasso ($\beta = $2.0)</t>
   </si>
 </sst>
 </file>

</xml_diff>